<commit_message>
Sort panel members by name
</commit_message>
<xml_diff>
--- a/ind-IRs-to-common-shocks.xlsx
+++ b/ind-IRs-to-common-shocks.xlsx
@@ -957,797 +957,797 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Russia</t>
+          <t>Belarus</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.01247208884926686</v>
+        <v>-0.0105328426116115</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.00259761964084626</v>
+        <v>-0.001591730123362439</v>
       </c>
       <c r="D3" t="n">
-        <v>0.002638595304687448</v>
+        <v>0.002781100568545389</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0009920467579371678</v>
+        <v>0.0009889901927044075</v>
       </c>
       <c r="F3" t="n">
-        <v>0.001216174927293032</v>
+        <v>0.0008251809354941366</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0002624441670718364</v>
+        <v>0.0001040556447082739</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.0006720277498249276</v>
+        <v>-0.0003219082230902691</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.0004875059774716816</v>
+        <v>-0.0003558014653627363</v>
       </c>
       <c r="J3" t="n">
-        <v>-8.083789496883309e-05</v>
+        <v>-0.0002409824487244205</v>
       </c>
       <c r="K3" t="n">
-        <v>9.176121959758774e-05</v>
+        <v>0.0001066981116065365</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0001698980105675226</v>
+        <v>0.000371545589442316</v>
       </c>
       <c r="M3" t="n">
-        <v>-3.311562280129565e-05</v>
+        <v>-3.263166176604545e-05</v>
       </c>
       <c r="N3" t="n">
-        <v>-1.537541308267224e-05</v>
+        <v>-0.0002227923017295831</v>
       </c>
       <c r="O3" t="n">
-        <v>1.431132176642492e-05</v>
+        <v>1.467603016123097e-05</v>
       </c>
       <c r="P3" t="n">
-        <v>2.286913359563256e-05</v>
+        <v>0.0002208563799336105</v>
       </c>
       <c r="Q3" t="n">
-        <v>-9.53394647484344e-05</v>
+        <v>-7.329563926958971e-05</v>
       </c>
       <c r="R3" t="n">
-        <v>0.0002002638726802537</v>
+        <v>-0.0002136004875584928</v>
       </c>
       <c r="S3" t="n">
-        <v>-2.213630224083552e-05</v>
+        <v>0.0002795464962101029</v>
       </c>
       <c r="T3" t="n">
-        <v>-6.800807606188626e-05</v>
+        <v>-9.731904729197263e-05</v>
       </c>
       <c r="U3" t="n">
-        <v>-9.741205056791617e-05</v>
+        <v>1.509134090039513e-05</v>
       </c>
       <c r="V3" t="n">
-        <v>2.798086190531927e-05</v>
+        <v>-4.341560873233935e-05</v>
       </c>
       <c r="W3" t="n">
-        <v>8.424003184928677e-06</v>
+        <v>0.0001896602359987792</v>
       </c>
       <c r="X3" t="n">
-        <v>1.520301477943099e-05</v>
+        <v>-0.0001128052801827177</v>
       </c>
       <c r="Y3" t="n">
-        <v>-5.812359905015329e-05</v>
+        <v>-1.930979936560755e-05</v>
       </c>
       <c r="Z3" t="n">
-        <v>4.525870483142159e-05</v>
+        <v>-3.746297936950324e-05</v>
       </c>
       <c r="AA3" t="n">
-        <v>4.31399635195741e-06</v>
+        <v>0.0001625998209002425</v>
       </c>
       <c r="AB3" t="n">
-        <v>2.254414589747095e-06</v>
+        <v>-8.716584943677695e-05</v>
       </c>
       <c r="AC3" t="n">
-        <v>-5.993076396724966e-05</v>
+        <v>-3.366824568357838e-05</v>
       </c>
       <c r="AD3" t="n">
-        <v>4.564605490101856e-05</v>
+        <v>-2.117554918964954e-05</v>
       </c>
       <c r="AE3" t="n">
-        <v>8.175044173947464e-06</v>
+        <v>0.0001369486533356425</v>
       </c>
       <c r="AF3" t="n">
-        <v>5.593691593324939e-06</v>
+        <v>-7.491299518346499e-05</v>
       </c>
       <c r="AG3" t="n">
-        <v>-5.75028671031397e-05</v>
+        <v>-4.301070535103594e-05</v>
       </c>
       <c r="AH3" t="n">
-        <v>-0.001256261703832377</v>
+        <v>6.922966840751045e-05</v>
       </c>
       <c r="AI3" t="n">
-        <v>-0.0008740648352823547</v>
+        <v>-0.00139204523599051</v>
       </c>
       <c r="AJ3" t="n">
-        <v>-7.418262798252811e-05</v>
+        <v>-0.0002764118114474998</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.0003027655472340206</v>
+        <v>0.0008689729013129036</v>
       </c>
       <c r="AL3" t="n">
-        <v>-0.0005449009143138616</v>
+        <v>-4.82917711103161e-05</v>
       </c>
       <c r="AM3" t="n">
-        <v>-0.0001984661406391989</v>
+        <v>-0.001089740157320466</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.0002101150711138262</v>
+        <v>9.352962252624129e-06</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.0003614353137033742</v>
+        <v>0.0008405020721209984</v>
       </c>
       <c r="AP3" t="n">
-        <v>-0.0005285302493241101</v>
+        <v>-3.110470959192759e-05</v>
       </c>
       <c r="AQ3" t="n">
-        <v>-0.0002020825545661648</v>
+        <v>-0.0009672034863833042</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.0002347523294704575</v>
+        <v>4.663768791512893e-05</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.0004065816175649672</v>
+        <v>0.0008359305916588565</v>
       </c>
       <c r="AT3" t="n">
-        <v>-0.0004701207687498053</v>
+        <v>-3.11425526109388e-05</v>
       </c>
       <c r="AU3" t="n">
-        <v>-0.0001832008749232752</v>
+        <v>-0.0008892505361840841</v>
       </c>
       <c r="AV3" t="n">
-        <v>0.0002286744828867091</v>
+        <v>7.275083295747981e-05</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.0003994082600885816</v>
+        <v>0.0008020982123507638</v>
       </c>
       <c r="AX3" t="n">
-        <v>-0.0004548468475511107</v>
+        <v>-0.0007161689681290952</v>
       </c>
       <c r="AY3" t="n">
-        <v>0.0001590320777461168</v>
+        <v>9.019029852591205e-05</v>
       </c>
       <c r="AZ3" t="n">
-        <v>9.964096594063287e-05</v>
+        <v>0.0001806603079946683</v>
       </c>
       <c r="BA3" t="n">
-        <v>6.237090350537208e-05</v>
+        <v>5.589424373861232e-05</v>
       </c>
       <c r="BB3" t="n">
-        <v>-0.0004074161715356444</v>
+        <v>-0.0005702834516113524</v>
       </c>
       <c r="BC3" t="n">
-        <v>0.0001728257074874928</v>
+        <v>0.0001245434197904944</v>
       </c>
       <c r="BD3" t="n">
-        <v>0.0001177684775808738</v>
+        <v>0.000245145031996731</v>
       </c>
       <c r="BE3" t="n">
-        <v>7.989876589982197e-05</v>
+        <v>4.683134062024944e-05</v>
       </c>
       <c r="BF3" t="n">
-        <v>-0.0003838305218304846</v>
+        <v>-0.0004846546244905359</v>
       </c>
       <c r="BG3" t="n">
-        <v>0.0001703822668606232</v>
+        <v>0.0001225657856856439</v>
       </c>
       <c r="BH3" t="n">
-        <v>0.0001195045992095789</v>
+        <v>0.0002679237466539825</v>
       </c>
       <c r="BI3" t="n">
-        <v>8.351151675609915e-05</v>
+        <v>2.545272026641084e-05</v>
       </c>
       <c r="BJ3" t="n">
-        <v>-0.0003702745382049986</v>
+        <v>-0.0004278095673335058</v>
       </c>
       <c r="BK3" t="n">
-        <v>0.0001623778177596557</v>
+        <v>0.0001134194752055613</v>
       </c>
       <c r="BL3" t="n">
-        <v>0.0001179953505449426</v>
+        <v>0.0002736518524534749</v>
       </c>
       <c r="BM3" t="n">
-        <v>8.510404194021317e-05</v>
+        <v>3.394126012969395e-06</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Croatia</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.01340447763710962</v>
+        <v>-0.00335437437461476</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.002355338807092421</v>
+        <v>-0.0008066426345402565</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00322439867123357</v>
+        <v>0.0004722323401855299</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002426717057127414</v>
+        <v>0.0002873251635292895</v>
       </c>
       <c r="F4" t="n">
-        <v>0.001887976999661214</v>
+        <v>-9.126100083625855e-05</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.0003278294362085113</v>
+        <v>-4.420483487031786e-05</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.001287366023375286</v>
+        <v>4.066278080620381e-05</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.0007235393475737337</v>
+        <v>2.89542649134531e-05</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.0001637276566844221</v>
+        <v>-7.15650083485053e-05</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0003002207761600925</v>
+        <v>3.395968285659243e-07</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0004512114653947258</v>
+        <v>4.74042660901004e-05</v>
       </c>
       <c r="M4" t="n">
-        <v>0.000145341055877901</v>
+        <v>2.185441467076684e-05</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.0001924428150873172</v>
+        <v>-6.458426082469765e-05</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.0002036959223106572</v>
+        <v>-3.080064153293987e-06</v>
       </c>
       <c r="P4" t="n">
-        <v>6.880876760420681e-06</v>
+        <v>4.273662903284871e-05</v>
       </c>
       <c r="Q4" t="n">
-        <v>7.402380924838596e-05</v>
+        <v>2.05613342774975e-05</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.0001527398952259301</v>
+        <v>2.577434633176392e-05</v>
       </c>
       <c r="S4" t="n">
-        <v>-2.532193754156739e-06</v>
+        <v>1.207828838857885e-05</v>
       </c>
       <c r="T4" t="n">
-        <v>2.53106462210255e-05</v>
+        <v>-1.6172626606111e-05</v>
       </c>
       <c r="U4" t="n">
-        <v>0.0001133850690655301</v>
+        <v>-3.147990604941173e-05</v>
       </c>
       <c r="V4" t="n">
-        <v>2.352973594153677e-05</v>
+        <v>2.606441380487036e-05</v>
       </c>
       <c r="W4" t="n">
-        <v>-4.343228892780173e-05</v>
+        <v>1.94884449295365e-05</v>
       </c>
       <c r="X4" t="n">
-        <v>-3.66711716029418e-05</v>
+        <v>-1.275402668232363e-05</v>
       </c>
       <c r="Y4" t="n">
-        <v>5.353740118096418e-05</v>
+        <v>-2.885817811889236e-05</v>
       </c>
       <c r="Z4" t="n">
-        <v>1.18837169731875e-05</v>
+        <v>2.090427119761166e-05</v>
       </c>
       <c r="AA4" t="n">
-        <v>-3.433103537243998e-05</v>
+        <v>1.837150324103578e-05</v>
       </c>
       <c r="AB4" t="n">
-        <v>-1.24471847216441e-05</v>
+        <v>-1.063517001009228e-05</v>
       </c>
       <c r="AC4" t="n">
-        <v>5.539884354176578e-05</v>
+        <v>-2.54909706797644e-05</v>
       </c>
       <c r="AD4" t="n">
-        <v>1.106631616026092e-05</v>
+        <v>1.702891213367311e-05</v>
       </c>
       <c r="AE4" t="n">
-        <v>-4.763365750305478e-05</v>
+        <v>1.70872594737281e-05</v>
       </c>
       <c r="AF4" t="n">
-        <v>-1.754831882644246e-05</v>
+        <v>-8.869185596644911e-06</v>
       </c>
       <c r="AG4" t="n">
-        <v>5.322401685014712e-05</v>
+        <v>-2.253737575754608e-05</v>
       </c>
       <c r="AH4" t="n">
-        <v>-0.0006445950341095861</v>
+        <v>-0.0002411417879041685</v>
       </c>
       <c r="AI4" t="n">
-        <v>-0.0009917877890339274</v>
+        <v>-0.0004190048641971001</v>
       </c>
       <c r="AJ4" t="n">
-        <v>-0.0003990007450472555</v>
+        <v>5.485339659105089e-06</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.0004213896295895422</v>
+        <v>6.708328221030322e-05</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.0001223980526670682</v>
+        <v>0.0001402112550110006</v>
       </c>
       <c r="AM4" t="n">
-        <v>-0.0005347839501926861</v>
+        <v>-0.000204432363883603</v>
       </c>
       <c r="AN4" t="n">
-        <v>-0.0002906075543669415</v>
+        <v>-2.39430205072122e-06</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.0003409657801087236</v>
+        <v>5.241781308684986e-05</v>
       </c>
       <c r="AP4" t="n">
-        <v>6.665278783972634e-05</v>
+        <v>0.0001241187712102378</v>
       </c>
       <c r="AQ4" t="n">
-        <v>-0.0005087126296724283</v>
+        <v>-0.0001639900691221224</v>
       </c>
       <c r="AR4" t="n">
-        <v>-0.0001931702640664422</v>
+        <v>-9.850988506498726e-06</v>
       </c>
       <c r="AS4" t="n">
-        <v>0.0004480675282011276</v>
+        <v>4.970256617702023e-05</v>
       </c>
       <c r="AT4" t="n">
-        <v>0.0001428949139659717</v>
+        <v>0.0001076672888324608</v>
       </c>
       <c r="AU4" t="n">
-        <v>-0.0004978622469339363</v>
+        <v>-0.0001362905198395821</v>
       </c>
       <c r="AV4" t="n">
-        <v>-0.0002056882089594981</v>
+        <v>-1.720336301951457e-05</v>
       </c>
       <c r="AW4" t="n">
-        <v>0.0004563483158026895</v>
+        <v>4.585436462528876e-05</v>
       </c>
       <c r="AX4" t="n">
-        <v>0.0004214351822502868</v>
+        <v>-0.0001140659011306308</v>
       </c>
       <c r="AY4" t="n">
-        <v>-1.547978295835814e-05</v>
+        <v>5.340985556044578e-05</v>
       </c>
       <c r="AZ4" t="n">
-        <v>-0.0001443716367741423</v>
+        <v>3.156822130307982e-05</v>
       </c>
       <c r="BA4" t="n">
-        <v>-2.638259381156993e-07</v>
+        <v>9.012890604214104e-06</v>
       </c>
       <c r="BB4" t="n">
-        <v>0.0003422853571893834</v>
+        <v>-9.132289206470997e-05</v>
       </c>
       <c r="BC4" t="n">
-        <v>-5.335058938248978e-06</v>
+        <v>4.495103448493151e-05</v>
       </c>
       <c r="BD4" t="n">
-        <v>-0.000212150833987332</v>
+        <v>3.312643677395521e-05</v>
       </c>
       <c r="BE4" t="n">
-        <v>-7.735295122618524e-06</v>
+        <v>8.1972033277875e-06</v>
       </c>
       <c r="BF4" t="n">
-        <v>0.0003027560045743789</v>
+        <v>-7.795250168361567e-05</v>
       </c>
       <c r="BG4" t="n">
-        <v>2.742089693508704e-06</v>
+        <v>3.487661066984684e-05</v>
       </c>
       <c r="BH4" t="n">
-        <v>-0.0002440734339955185</v>
+        <v>3.208935592700033e-05</v>
       </c>
       <c r="BI4" t="n">
-        <v>-1.175711276249527e-05</v>
+        <v>7.201325434242603e-06</v>
       </c>
       <c r="BJ4" t="n">
-        <v>0.0002877287258341529</v>
+        <v>-6.687224886780032e-05</v>
       </c>
       <c r="BK4" t="n">
-        <v>1.028771701435968e-05</v>
+        <v>2.665973125419076e-05</v>
       </c>
       <c r="BL4" t="n">
-        <v>-0.0002618345269249247</v>
+        <v>3.044299607686966e-05</v>
       </c>
       <c r="BM4" t="n">
-        <v>-1.735702302297607e-05</v>
+        <v>6.511513562445282e-06</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Belarus</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.0105328426116115</v>
+        <v>-0.011542484778405</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.001591730123362439</v>
+        <v>-0.0027841987228592</v>
       </c>
       <c r="D5" t="n">
-        <v>0.002781100568545389</v>
+        <v>0.002301219534904933</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0009889901927044075</v>
+        <v>0.002141423800213681</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0008251809354941366</v>
+        <v>0.0005921746221370563</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0001040556447082739</v>
+        <v>-0.0002239874546006131</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.0003219082230902691</v>
+        <v>-0.0005088516293779625</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.0003558014653627363</v>
+        <v>-0.000129993192646906</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.0002409824487244205</v>
+        <v>-4.701432280172318e-05</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0001066981116065365</v>
+        <v>0.0001531824945621654</v>
       </c>
       <c r="L5" t="n">
-        <v>0.000371545589442316</v>
+        <v>3.274053524201541e-05</v>
       </c>
       <c r="M5" t="n">
-        <v>-3.263166176604545e-05</v>
+        <v>4.693302467361065e-05</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.0002227923017295831</v>
+        <v>-9.884565423113951e-05</v>
       </c>
       <c r="O5" t="n">
-        <v>1.467603016123097e-05</v>
+        <v>2.750999595005686e-05</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0002208563799336105</v>
+        <v>-9.185148750313485e-06</v>
       </c>
       <c r="Q5" t="n">
-        <v>-7.329563926958971e-05</v>
+        <v>4.277207210603171e-05</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.0002136004875584928</v>
+        <v>2.927095768189455e-05</v>
       </c>
       <c r="S5" t="n">
-        <v>0.0002795464962101029</v>
+        <v>-2.827039696738755e-05</v>
       </c>
       <c r="T5" t="n">
-        <v>-9.731904729197263e-05</v>
+        <v>7.199866608422091e-05</v>
       </c>
       <c r="U5" t="n">
-        <v>1.509134090039513e-05</v>
+        <v>-9.343602087913911e-05</v>
       </c>
       <c r="V5" t="n">
-        <v>-4.341560873233935e-05</v>
+        <v>9.682269192847693e-05</v>
       </c>
       <c r="W5" t="n">
-        <v>0.0001896602359987792</v>
+        <v>-1.716045447717832e-05</v>
       </c>
       <c r="X5" t="n">
-        <v>-0.0001128052801827177</v>
+        <v>1.465288959506389e-05</v>
       </c>
       <c r="Y5" t="n">
-        <v>-1.930979936560755e-05</v>
+        <v>-9.123390297232556e-05</v>
       </c>
       <c r="Z5" t="n">
-        <v>-3.746297936950324e-05</v>
+        <v>8.084489299605205e-05</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.0001625998209002425</v>
+        <v>-4.154051843094286e-06</v>
       </c>
       <c r="AB5" t="n">
-        <v>-8.716584943677695e-05</v>
+        <v>7.852982629980063e-06</v>
       </c>
       <c r="AC5" t="n">
-        <v>-3.366824568357838e-05</v>
+        <v>-7.402035332472659e-05</v>
       </c>
       <c r="AD5" t="n">
-        <v>-2.117554918964954e-05</v>
+        <v>6.795508548853205e-05</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.0001369486533356425</v>
+        <v>-1.682158804288142e-08</v>
       </c>
       <c r="AF5" t="n">
-        <v>-7.491299518346499e-05</v>
+        <v>-6.750677671356846e-07</v>
       </c>
       <c r="AG5" t="n">
-        <v>-4.301070535103594e-05</v>
+        <v>-6.043109658519211e-05</v>
       </c>
       <c r="AH5" t="n">
-        <v>6.922966840751045e-05</v>
+        <v>0.0004655613126746067</v>
       </c>
       <c r="AI5" t="n">
-        <v>-0.00139204523599051</v>
+        <v>-0.001077245638825984</v>
       </c>
       <c r="AJ5" t="n">
-        <v>-0.0002764118114474998</v>
+        <v>-0.0002277071482222299</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.0008689729013129036</v>
+        <v>-1.152386659833562e-05</v>
       </c>
       <c r="AL5" t="n">
-        <v>-4.82917711103161e-05</v>
+        <v>0.0004122535513756173</v>
       </c>
       <c r="AM5" t="n">
-        <v>-0.001089740157320466</v>
+        <v>-0.0003943887749922669</v>
       </c>
       <c r="AN5" t="n">
-        <v>9.352962252624129e-06</v>
+        <v>0.0001073968974709503</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.0008405020721209984</v>
+        <v>4.760599359832952e-05</v>
       </c>
       <c r="AP5" t="n">
-        <v>-3.110470959192759e-05</v>
+        <v>0.0002444628182660329</v>
       </c>
       <c r="AQ5" t="n">
-        <v>-0.0009672034863833042</v>
+        <v>-0.0004010216038687176</v>
       </c>
       <c r="AR5" t="n">
-        <v>4.663768791512893e-05</v>
+        <v>7.133973243068994e-05</v>
       </c>
       <c r="AS5" t="n">
-        <v>0.0008359305916588565</v>
+        <v>9.283727904658188e-05</v>
       </c>
       <c r="AT5" t="n">
-        <v>-3.11425526109388e-05</v>
+        <v>0.000203597807405603</v>
       </c>
       <c r="AU5" t="n">
-        <v>-0.0008892505361840841</v>
+        <v>-0.0003438838005736204</v>
       </c>
       <c r="AV5" t="n">
-        <v>7.275083295747981e-05</v>
+        <v>5.113010050716808e-05</v>
       </c>
       <c r="AW5" t="n">
-        <v>0.0008020982123507638</v>
+        <v>0.0001051058543844435</v>
       </c>
       <c r="AX5" t="n">
-        <v>-0.0007161689681290952</v>
+        <v>-0.0006748241701191055</v>
       </c>
       <c r="AY5" t="n">
-        <v>9.019029852591205e-05</v>
+        <v>0.0003646681919455549</v>
       </c>
       <c r="AZ5" t="n">
-        <v>0.0001806603079946683</v>
+        <v>0.0001947409761920276</v>
       </c>
       <c r="BA5" t="n">
-        <v>5.589424373861232e-05</v>
+        <v>1.555615497352041e-05</v>
       </c>
       <c r="BB5" t="n">
-        <v>-0.0005702834516113524</v>
+        <v>-0.0005526652965100798</v>
       </c>
       <c r="BC5" t="n">
-        <v>0.0001245434197904944</v>
+        <v>0.0003358789764750778</v>
       </c>
       <c r="BD5" t="n">
-        <v>0.000245145031996731</v>
+        <v>0.0002047805413076573</v>
       </c>
       <c r="BE5" t="n">
-        <v>4.683134062024944e-05</v>
+        <v>-3.051307395688114e-05</v>
       </c>
       <c r="BF5" t="n">
-        <v>-0.0004846546244905359</v>
+        <v>-0.0004725934012406942</v>
       </c>
       <c r="BG5" t="n">
-        <v>0.0001225657856856439</v>
+        <v>0.0003004052208258338</v>
       </c>
       <c r="BH5" t="n">
-        <v>0.0002679237466539825</v>
+        <v>0.0002014713609796367</v>
       </c>
       <c r="BI5" t="n">
-        <v>2.545272026641084e-05</v>
+        <v>-6.477199607115762e-05</v>
       </c>
       <c r="BJ5" t="n">
-        <v>-0.0004278095673335058</v>
+        <v>-0.0004043887779086576</v>
       </c>
       <c r="BK5" t="n">
-        <v>0.0001134194752055613</v>
+        <v>0.0002718675192607903</v>
       </c>
       <c r="BL5" t="n">
-        <v>0.0002736518524534749</v>
+        <v>0.0001930787607812153</v>
       </c>
       <c r="BM5" t="n">
-        <v>3.394126012969395e-06</v>
+        <v>-8.979418418545809e-05</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.006817454136490148</v>
+        <v>0.000723789783913524</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.002824349490402249</v>
+        <v>5.337551159147233e-05</v>
       </c>
       <c r="D6" t="n">
-        <v>0.001908746294458336</v>
+        <v>3.512206109297829e-06</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0009183449647471652</v>
+        <v>1.190632137910052e-09</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00141196092540656</v>
+        <v>-1.397434351554525e-07</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.0004708797051527248</v>
+        <v>-8.503050745970242e-08</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.0007148733136847689</v>
+        <v>-4.612112489947368e-08</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.0009767874470779463</v>
+        <v>-2.464715724395904e-08</v>
       </c>
       <c r="J6" t="n">
-        <v>0.000503078560413692</v>
+        <v>-1.314422907094899e-08</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0001313498933376699</v>
+        <v>-7.007726464997723e-09</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0005337048892192508</v>
+        <v>-3.735952969871812e-09</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.000473385020645305</v>
+        <v>-1.991696498388372e-09</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0002195642953954438</v>
+        <v>-1.061804514380514e-09</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.0003286676193286278</v>
+        <v>-5.660645079103802e-10</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0002696613894595519</v>
+        <v>-3.017777920861969e-10</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.0003676975644150233</v>
+        <v>-1.608824335711787e-10</v>
       </c>
       <c r="R6" t="n">
-        <v>0.001216055286032424</v>
+        <v>-1.459646503581326e-05</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.0002795745100847273</v>
+        <v>5.720428061091758e-06</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.0005691126335926916</v>
+        <v>4.062565534814152e-06</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.0005830951630117643</v>
+        <v>2.241805399288638e-06</v>
       </c>
       <c r="V6" t="n">
-        <v>0.0001573277791492809</v>
+        <v>1.200841944617782e-06</v>
       </c>
       <c r="W6" t="n">
-        <v>0.0002197927588826258</v>
+        <v>6.406151719115035e-07</v>
       </c>
       <c r="X6" t="n">
-        <v>0.0002600650604791017</v>
+        <v>3.415539922658561e-07</v>
       </c>
       <c r="Y6" t="n">
-        <v>-0.0003018505284590701</v>
+        <v>1.820901511690555e-07</v>
       </c>
       <c r="Z6" t="n">
-        <v>8.963026103253453e-05</v>
+        <v>9.707527159292597e-08</v>
       </c>
       <c r="AA6" t="n">
-        <v>-5.266494003405934e-05</v>
+        <v>5.175235032189647e-08</v>
       </c>
       <c r="AB6" t="n">
-        <v>6.847123617284079e-05</v>
+        <v>2.758998370569106e-08</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.000240644385097675</v>
+        <v>1.470864940538075e-08</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.0002165385274900791</v>
+        <v>7.841409718639324e-09</v>
       </c>
       <c r="AE6" t="n">
-        <v>2.065604119064575e-05</v>
+        <v>4.180377452911712e-09</v>
       </c>
       <c r="AF6" t="n">
-        <v>5.76281716373613e-05</v>
+        <v>2.228624223745305e-09</v>
       </c>
       <c r="AG6" t="n">
-        <v>-0.0002792229617869397</v>
+        <v>1.188114228092796e-09</v>
       </c>
       <c r="AH6" t="n">
-        <v>-0.001868834067770949</v>
+        <v>1.147046921577e-05</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.00116936493897521</v>
+        <v>1.244133414807385e-05</v>
       </c>
       <c r="AJ6" t="n">
-        <v>-0.0009875989338892117</v>
+        <v>7.10726108042742e-06</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.0006297560445297976</v>
+        <v>3.824595109534211e-06</v>
       </c>
       <c r="AL6" t="n">
-        <v>-0.001740714892398925</v>
+        <v>2.041622098937219e-06</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.001521490567209997</v>
+        <v>1.088620862882315e-06</v>
       </c>
       <c r="AN6" t="n">
-        <v>-0.0003756569660115169</v>
+        <v>5.803757417881756e-07</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.0006658859921988707</v>
+        <v>3.094084603084102e-07</v>
       </c>
       <c r="AP6" t="n">
-        <v>-0.001765616011150358</v>
+        <v>1.649505459949991e-07</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.001396342869298769</v>
+        <v>8.793770734610781e-08</v>
       </c>
       <c r="AR6" t="n">
-        <v>-0.0004281498384506311</v>
+        <v>4.688095966625943e-08</v>
       </c>
       <c r="AS6" t="n">
-        <v>0.000690976793022293</v>
+        <v>2.499296861810585e-08</v>
       </c>
       <c r="AT6" t="n">
-        <v>-0.001603205660755752</v>
+        <v>1.332414020586062e-08</v>
       </c>
       <c r="AU6" t="n">
-        <v>0.001383436954469312</v>
+        <v>7.10330633017084e-09</v>
       </c>
       <c r="AV6" t="n">
-        <v>-0.0004561865280287833</v>
+        <v>3.786883058827668e-09</v>
       </c>
       <c r="AW6" t="n">
-        <v>0.0006279972710057978</v>
+        <v>2.018846243512917e-09</v>
       </c>
       <c r="AX6" t="n">
-        <v>-0.001481409670242136</v>
+        <v>-0.0001861341407346146</v>
       </c>
       <c r="AY6" t="n">
-        <v>0.0008190640786055996</v>
+        <v>-9.94879078076802e-05</v>
       </c>
       <c r="AZ6" t="n">
-        <v>0.0004753683442458637</v>
+        <v>-5.305782341219773e-05</v>
       </c>
       <c r="BA6" t="n">
-        <v>1.469140024617399e-05</v>
+        <v>-2.828739652716761e-05</v>
       </c>
       <c r="BB6" t="n">
-        <v>-0.001325822076303825</v>
+        <v>-1.508055941462212e-05</v>
       </c>
       <c r="BC6" t="n">
-        <v>0.0007759242408129056</v>
+        <v>-8.039688858987654e-06</v>
       </c>
       <c r="BD6" t="n">
-        <v>0.0003994069690658975</v>
+        <v>-4.286083755819537e-06</v>
       </c>
       <c r="BE6" t="n">
-        <v>5.369274018256173e-05</v>
+        <v>-2.284977943288148e-06</v>
       </c>
       <c r="BF6" t="n">
-        <v>-0.001201982913856476</v>
+        <v>-1.218157275696945e-06</v>
       </c>
       <c r="BG6" t="n">
-        <v>0.0007877262001044842</v>
+        <v>-6.494185858975684e-07</v>
       </c>
       <c r="BH6" t="n">
-        <v>0.000353730878009706</v>
+        <v>-3.462151464178403e-07</v>
       </c>
       <c r="BI6" t="n">
-        <v>1.644672141746335e-05</v>
+        <v>-1.845726780943726e-07</v>
       </c>
       <c r="BJ6" t="n">
-        <v>-0.00113987776187163</v>
+        <v>-9.839856473981063e-08</v>
       </c>
       <c r="BK6" t="n">
-        <v>0.0007840810099507797</v>
+        <v>-5.245780492980071e-08</v>
       </c>
       <c r="BL6" t="n">
-        <v>0.0003212902493106685</v>
+        <v>-2.796607151058687e-08</v>
       </c>
       <c r="BM6" t="n">
-        <v>3.116573100228982e-06</v>
+        <v>-1.490914758598564e-08</v>
       </c>
     </row>
     <row r="7">
@@ -1952,2389 +1952,2389 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.01396051345341312</v>
+        <v>-0.01129781201639208</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.002158976928164716</v>
+        <v>-0.003750672387688495</v>
       </c>
       <c r="D8" t="n">
-        <v>0.003116494644317403</v>
+        <v>0.002158064106622794</v>
       </c>
       <c r="E8" t="n">
-        <v>0.002192089939542271</v>
+        <v>0.001491596504195784</v>
       </c>
       <c r="F8" t="n">
-        <v>0.001487031770628142</v>
+        <v>-0.000304332099853026</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.0005671184083243523</v>
+        <v>-0.0004789439704000658</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.001265750274180509</v>
+        <v>-1.282572921602585e-05</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.0004040237840816947</v>
+        <v>0.0001314598047460085</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0002912140634641279</v>
+        <v>3.042860567636523e-05</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0002589337520266327</v>
+        <v>-3.057543079262467e-05</v>
       </c>
       <c r="L8" t="n">
-        <v>1.566441433938606e-05</v>
+        <v>-1.476077933801122e-05</v>
       </c>
       <c r="M8" t="n">
-        <v>-4.385363863131341e-06</v>
+        <v>5.542680556365517e-06</v>
       </c>
       <c r="N8" t="n">
-        <v>7.323272804820467e-05</v>
+        <v>5.263039408915522e-06</v>
       </c>
       <c r="O8" t="n">
-        <v>-8.87079396244289e-05</v>
+        <v>-4.763702841943097e-07</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.000152722109937445</v>
+        <v>-1.57025395022482e-06</v>
       </c>
       <c r="Q8" t="n">
-        <v>3.810932301609093e-05</v>
+        <v>-1.873661431387835e-07</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.0002139685894622191</v>
+        <v>-0.0005645770715270606</v>
       </c>
       <c r="S8" t="n">
-        <v>8.76301931360159e-05</v>
+        <v>0.0003021183309953039</v>
       </c>
       <c r="T8" t="n">
-        <v>0.0001226768641403904</v>
+        <v>0.0003742726520876313</v>
       </c>
       <c r="U8" t="n">
-        <v>8.401365196164062e-06</v>
+        <v>-1.944201629540598e-05</v>
       </c>
       <c r="V8" t="n">
-        <v>-7.700029338406603e-05</v>
+        <v>-0.0001041285260479386</v>
       </c>
       <c r="W8" t="n">
-        <v>4.260461600450783e-05</v>
+        <v>-1.664257147428668e-05</v>
       </c>
       <c r="X8" t="n">
-        <v>3.739630515009481e-05</v>
+        <v>2.594155761011319e-05</v>
       </c>
       <c r="Y8" t="n">
-        <v>-1.433675737670788e-05</v>
+        <v>9.913737467874904e-06</v>
       </c>
       <c r="Z8" t="n">
-        <v>-7.584249789264906e-05</v>
+        <v>-5.226207041402771e-06</v>
       </c>
       <c r="AA8" t="n">
-        <v>5.330356006443507e-05</v>
+        <v>-3.843943136011078e-06</v>
       </c>
       <c r="AB8" t="n">
-        <v>4.33782974644208e-05</v>
+        <v>6.780751532796277e-07</v>
       </c>
       <c r="AC8" t="n">
-        <v>-1.264869908348796e-05</v>
+        <v>1.214184479316006e-06</v>
       </c>
       <c r="AD8" t="n">
-        <v>-7.686769145436746e-05</v>
+        <v>5.821836531727477e-08</v>
       </c>
       <c r="AE8" t="n">
-        <v>4.664935348882033e-05</v>
+        <v>-3.279285778987807e-07</v>
       </c>
       <c r="AF8" t="n">
-        <v>3.738901090664405e-05</v>
+        <v>-8.32643006229574e-08</v>
       </c>
       <c r="AG8" t="n">
-        <v>-8.765036897952209e-06</v>
+        <v>7.477224194626928e-08</v>
       </c>
       <c r="AH8" t="n">
-        <v>-0.0004521498910312746</v>
+        <v>-0.0004656474233849604</v>
       </c>
       <c r="AI8" t="n">
-        <v>-0.0002621452860699645</v>
+        <v>-0.0002385255865849153</v>
       </c>
       <c r="AJ8" t="n">
-        <v>8.715320815176587e-05</v>
+        <v>2.078972274810803e-05</v>
       </c>
       <c r="AK8" t="n">
-        <v>1.026038065505312e-05</v>
+        <v>7.588071470848605e-05</v>
       </c>
       <c r="AL8" t="n">
-        <v>-0.0002313720854066402</v>
+        <v>7.818379039415234e-06</v>
       </c>
       <c r="AM8" t="n">
-        <v>-5.848951006772484e-07</v>
+        <v>-1.930261675328244e-05</v>
       </c>
       <c r="AN8" t="n">
-        <v>0.0001723622650875499</v>
+        <v>-6.211235135160237e-06</v>
       </c>
       <c r="AO8" t="n">
-        <v>2.30397345042161e-05</v>
+        <v>4.150944957357818e-06</v>
       </c>
       <c r="AP8" t="n">
-        <v>-0.0002305859267309316</v>
+        <v>2.582219085262826e-06</v>
       </c>
       <c r="AQ8" t="n">
-        <v>-7.676493391619687e-06</v>
+        <v>-6.335220994128412e-07</v>
       </c>
       <c r="AR8" t="n">
-        <v>0.0001707335949599321</v>
+        <v>-8.522534149296273e-07</v>
       </c>
       <c r="AS8" t="n">
-        <v>4.288379770602197e-05</v>
+        <v>3.291636492048402e-09</v>
       </c>
       <c r="AT8" t="n">
-        <v>-0.0002023575145804124</v>
+        <v>2.391831361992723e-07</v>
       </c>
       <c r="AU8" t="n">
-        <v>-2.8840304993375e-06</v>
+        <v>4.792837243806067e-08</v>
       </c>
       <c r="AV8" t="n">
-        <v>0.0001533864352618064</v>
+        <v>-5.715229777192262e-08</v>
       </c>
       <c r="AW8" t="n">
-        <v>3.983948602330101e-05</v>
+        <v>-2.508563611103822e-08</v>
       </c>
       <c r="AX8" t="n">
-        <v>0.0001594425700768687</v>
+        <v>8.65852086728806e-05</v>
       </c>
       <c r="AY8" t="n">
-        <v>-6.271483753174544e-05</v>
+        <v>-1.985081832440554e-05</v>
       </c>
       <c r="AZ8" t="n">
-        <v>-2.745786114883133e-05</v>
+        <v>2.096914348264309e-05</v>
       </c>
       <c r="BA8" t="n">
-        <v>-2.58022146100628e-05</v>
+        <v>2.765628338221829e-06</v>
       </c>
       <c r="BB8" t="n">
-        <v>0.0001395704320665578</v>
+        <v>-3.397483427823654e-06</v>
       </c>
       <c r="BC8" t="n">
-        <v>-6.944265506908824e-05</v>
+        <v>-1.855720689008862e-06</v>
       </c>
       <c r="BD8" t="n">
-        <v>-2.65116009081893e-05</v>
+        <v>6.602654985352343e-07</v>
       </c>
       <c r="BE8" t="n">
-        <v>-3.2987028249834e-05</v>
+        <v>6.350025691244352e-07</v>
       </c>
       <c r="BF8" t="n">
-        <v>0.0001303618711053087</v>
+        <v>-5.084864263971351e-08</v>
       </c>
       <c r="BG8" t="n">
-        <v>-7.035803289000637e-05</v>
+        <v>-1.890377156836957e-07</v>
       </c>
       <c r="BH8" t="n">
-        <v>-2.062965602868131e-05</v>
+        <v>-2.416937281539293e-08</v>
       </c>
       <c r="BI8" t="n">
-        <v>-3.580223137803959e-05</v>
+        <v>4.792449340720134e-08</v>
       </c>
       <c r="BJ8" t="n">
-        <v>0.0001244436778162422</v>
+        <v>1.656174732145007e-08</v>
       </c>
       <c r="BK8" t="n">
-        <v>-6.983709384066289e-05</v>
+        <v>-1.003246554819092e-08</v>
       </c>
       <c r="BL8" t="n">
-        <v>-1.44794592640089e-05</v>
+        <v>-6.683544751776286e-09</v>
       </c>
       <c r="BM8" t="n">
-        <v>-3.804509305107701e-05</v>
+        <v>1.442717313373361e-09</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>CostaRica</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.00335437437461476</v>
+        <v>-0.004211389424389104</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.0008066426345402565</v>
+        <v>0.001801562945747068</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0004722323401855299</v>
+        <v>-0.0001451315792163281</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0002873251635292895</v>
+        <v>9.957940692377236e-05</v>
       </c>
       <c r="F9" t="n">
-        <v>-9.126100083625855e-05</v>
+        <v>-0.0002760248202494819</v>
       </c>
       <c r="G9" t="n">
-        <v>-4.420483487031786e-05</v>
+        <v>0.0002180040073599001</v>
       </c>
       <c r="H9" t="n">
-        <v>4.066278080620381e-05</v>
+        <v>-0.0001393266924149872</v>
       </c>
       <c r="I9" t="n">
-        <v>2.89542649134531e-05</v>
+        <v>8.072696263516521e-05</v>
       </c>
       <c r="J9" t="n">
-        <v>-7.15650083485053e-05</v>
+        <v>-3.561899881855213e-05</v>
       </c>
       <c r="K9" t="n">
-        <v>3.395968285659243e-07</v>
+        <v>4.622352487852608e-05</v>
       </c>
       <c r="L9" t="n">
-        <v>4.74042660901004e-05</v>
+        <v>-7.459301091585917e-05</v>
       </c>
       <c r="M9" t="n">
-        <v>2.185441467076684e-05</v>
+        <v>5.194203606023637e-05</v>
       </c>
       <c r="N9" t="n">
-        <v>-6.458426082469765e-05</v>
+        <v>-9.764762860796175e-06</v>
       </c>
       <c r="O9" t="n">
-        <v>-3.080064153293987e-06</v>
+        <v>1.371188018495599e-05</v>
       </c>
       <c r="P9" t="n">
-        <v>4.273662903284871e-05</v>
+        <v>-4.089588735002298e-05</v>
       </c>
       <c r="Q9" t="n">
-        <v>2.05613342774975e-05</v>
+        <v>3.262767526185956e-05</v>
       </c>
       <c r="R9" t="n">
-        <v>2.577434633176392e-05</v>
+        <v>-3.324102987555109e-05</v>
       </c>
       <c r="S9" t="n">
-        <v>1.207828838857885e-05</v>
+        <v>-0.000140366223564028</v>
       </c>
       <c r="T9" t="n">
-        <v>-1.6172626606111e-05</v>
+        <v>7.004536453765569e-05</v>
       </c>
       <c r="U9" t="n">
-        <v>-3.147990604941173e-05</v>
+        <v>0.0002635139221584385</v>
       </c>
       <c r="V9" t="n">
-        <v>2.606441380487036e-05</v>
+        <v>-0.000271032375935618</v>
       </c>
       <c r="W9" t="n">
-        <v>1.94884449295365e-05</v>
+        <v>-4.945388129882832e-05</v>
       </c>
       <c r="X9" t="n">
-        <v>-1.275402668232363e-05</v>
+        <v>9.831184292090049e-05</v>
       </c>
       <c r="Y9" t="n">
-        <v>-2.885817811889236e-05</v>
+        <v>0.0001531048600238268</v>
       </c>
       <c r="Z9" t="n">
-        <v>2.090427119761166e-05</v>
+        <v>-0.0002017633582428767</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.837150324103578e-05</v>
+        <v>-2.005162282808896e-05</v>
       </c>
       <c r="AB9" t="n">
-        <v>-1.063517001009228e-05</v>
+        <v>9.090697051552346e-05</v>
       </c>
       <c r="AC9" t="n">
-        <v>-2.54909706797644e-05</v>
+        <v>7.603019569579213e-05</v>
       </c>
       <c r="AD9" t="n">
-        <v>1.702891213367311e-05</v>
+        <v>-0.0001384954403689712</v>
       </c>
       <c r="AE9" t="n">
-        <v>1.70872594737281e-05</v>
+        <v>-3.664265669874047e-06</v>
       </c>
       <c r="AF9" t="n">
-        <v>-8.869185596644911e-06</v>
+        <v>7.37236597418614e-05</v>
       </c>
       <c r="AG9" t="n">
-        <v>-2.253737575754608e-05</v>
+        <v>3.24313821898932e-05</v>
       </c>
       <c r="AH9" t="n">
-        <v>-0.0002411417879041685</v>
+        <v>-6.0283971876563e-05</v>
       </c>
       <c r="AI9" t="n">
-        <v>-0.0004190048641971001</v>
+        <v>4.57983784108557e-05</v>
       </c>
       <c r="AJ9" t="n">
-        <v>5.485339659105089e-06</v>
+        <v>-7.257117343298604e-05</v>
       </c>
       <c r="AK9" t="n">
-        <v>6.708328221030322e-05</v>
+        <v>7.780232546299756e-05</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.0001402112550110006</v>
+        <v>-3.453775738594633e-05</v>
       </c>
       <c r="AM9" t="n">
-        <v>-0.000204432363883603</v>
+        <v>1.223931131860855e-05</v>
       </c>
       <c r="AN9" t="n">
-        <v>-2.39430205072122e-06</v>
+        <v>-4.052653189961699e-05</v>
       </c>
       <c r="AO9" t="n">
-        <v>5.241781308684986e-05</v>
+        <v>5.197100213082437e-05</v>
       </c>
       <c r="AP9" t="n">
-        <v>0.0001241187712102378</v>
+        <v>-2.067277650406911e-05</v>
       </c>
       <c r="AQ9" t="n">
-        <v>-0.0001639900691221224</v>
+        <v>8.881540460746051e-07</v>
       </c>
       <c r="AR9" t="n">
-        <v>-9.850988506498726e-06</v>
+        <v>-1.934990446598109e-05</v>
       </c>
       <c r="AS9" t="n">
-        <v>4.970256617702023e-05</v>
+        <v>3.178063794509458e-05</v>
       </c>
       <c r="AT9" t="n">
-        <v>0.0001076672888324608</v>
+        <v>-1.287589334332308e-05</v>
       </c>
       <c r="AU9" t="n">
-        <v>-0.0001362905198395821</v>
+        <v>-2.908646027652812e-06</v>
       </c>
       <c r="AV9" t="n">
-        <v>-1.720336301951457e-05</v>
+        <v>-8.215139704254001e-06</v>
       </c>
       <c r="AW9" t="n">
-        <v>4.585436462528876e-05</v>
+        <v>1.93043816781864e-05</v>
       </c>
       <c r="AX9" t="n">
-        <v>-0.0001140659011306308</v>
+        <v>-0.0003221546823674668</v>
       </c>
       <c r="AY9" t="n">
-        <v>5.340985556044578e-05</v>
+        <v>8.038390210105508e-05</v>
       </c>
       <c r="AZ9" t="n">
-        <v>3.156822130307982e-05</v>
+        <v>8.531987829242041e-05</v>
       </c>
       <c r="BA9" t="n">
-        <v>9.012890604214104e-06</v>
+        <v>-9.750266313907187e-06</v>
       </c>
       <c r="BB9" t="n">
-        <v>-9.132289206470997e-05</v>
+        <v>-0.0001794106152369146</v>
       </c>
       <c r="BC9" t="n">
-        <v>4.495103448493151e-05</v>
+        <v>7.929059931092063e-05</v>
       </c>
       <c r="BD9" t="n">
-        <v>3.312643677395521e-05</v>
+        <v>7.1633850620545e-05</v>
       </c>
       <c r="BE9" t="n">
-        <v>8.1972033277875e-06</v>
+        <v>-2.559289378101197e-05</v>
       </c>
       <c r="BF9" t="n">
-        <v>-7.795250168361567e-05</v>
+        <v>-0.0001056178867479846</v>
       </c>
       <c r="BG9" t="n">
-        <v>3.487661066984684e-05</v>
+        <v>6.449376501011359e-05</v>
       </c>
       <c r="BH9" t="n">
-        <v>3.208935592700033e-05</v>
+        <v>4.891737162871557e-05</v>
       </c>
       <c r="BI9" t="n">
-        <v>7.201325434242603e-06</v>
+        <v>-3.117065958383373e-05</v>
       </c>
       <c r="BJ9" t="n">
-        <v>-6.687224886780032e-05</v>
+        <v>-6.190050581578163e-05</v>
       </c>
       <c r="BK9" t="n">
-        <v>2.665973125419076e-05</v>
+        <v>4.989416596359252e-05</v>
       </c>
       <c r="BL9" t="n">
-        <v>3.044299607686966e-05</v>
+        <v>3.042066366208748e-05</v>
       </c>
       <c r="BM9" t="n">
-        <v>6.511513562445282e-06</v>
+        <v>-2.969763515772696e-05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>CostaRica</t>
+          <t>Croatia</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.004211389424389104</v>
+        <v>-0.01340447763710962</v>
       </c>
       <c r="C10" t="n">
-        <v>0.001801562945747068</v>
+        <v>-0.002355338807092421</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.0001451315792163281</v>
+        <v>0.00322439867123357</v>
       </c>
       <c r="E10" t="n">
-        <v>9.957940692377236e-05</v>
+        <v>0.002426717057127414</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.0002760248202494819</v>
+        <v>0.001887976999661214</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0002180040073599001</v>
+        <v>-0.0003278294362085113</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.0001393266924149872</v>
+        <v>-0.001287366023375286</v>
       </c>
       <c r="I10" t="n">
-        <v>8.072696263516521e-05</v>
+        <v>-0.0007235393475737337</v>
       </c>
       <c r="J10" t="n">
-        <v>-3.561899881855213e-05</v>
+        <v>-0.0001637276566844221</v>
       </c>
       <c r="K10" t="n">
-        <v>4.622352487852608e-05</v>
+        <v>0.0003002207761600925</v>
       </c>
       <c r="L10" t="n">
-        <v>-7.459301091585917e-05</v>
+        <v>0.0004512114653947258</v>
       </c>
       <c r="M10" t="n">
-        <v>5.194203606023637e-05</v>
+        <v>0.000145341055877901</v>
       </c>
       <c r="N10" t="n">
-        <v>-9.764762860796175e-06</v>
+        <v>-0.0001924428150873172</v>
       </c>
       <c r="O10" t="n">
-        <v>1.371188018495599e-05</v>
+        <v>-0.0002036959223106572</v>
       </c>
       <c r="P10" t="n">
-        <v>-4.089588735002298e-05</v>
+        <v>6.880876760420681e-06</v>
       </c>
       <c r="Q10" t="n">
-        <v>3.262767526185956e-05</v>
+        <v>7.402380924838596e-05</v>
       </c>
       <c r="R10" t="n">
-        <v>-3.324102987555109e-05</v>
+        <v>-0.0001527398952259301</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.000140366223564028</v>
+        <v>-2.532193754156739e-06</v>
       </c>
       <c r="T10" t="n">
-        <v>7.004536453765569e-05</v>
+        <v>2.53106462210255e-05</v>
       </c>
       <c r="U10" t="n">
-        <v>0.0002635139221584385</v>
+        <v>0.0001133850690655301</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.000271032375935618</v>
+        <v>2.352973594153677e-05</v>
       </c>
       <c r="W10" t="n">
-        <v>-4.945388129882832e-05</v>
+        <v>-4.343228892780173e-05</v>
       </c>
       <c r="X10" t="n">
-        <v>9.831184292090049e-05</v>
+        <v>-3.66711716029418e-05</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.0001531048600238268</v>
+        <v>5.353740118096418e-05</v>
       </c>
       <c r="Z10" t="n">
-        <v>-0.0002017633582428767</v>
+        <v>1.18837169731875e-05</v>
       </c>
       <c r="AA10" t="n">
-        <v>-2.005162282808896e-05</v>
+        <v>-3.433103537243998e-05</v>
       </c>
       <c r="AB10" t="n">
-        <v>9.090697051552346e-05</v>
+        <v>-1.24471847216441e-05</v>
       </c>
       <c r="AC10" t="n">
-        <v>7.603019569579213e-05</v>
+        <v>5.539884354176578e-05</v>
       </c>
       <c r="AD10" t="n">
-        <v>-0.0001384954403689712</v>
+        <v>1.106631616026092e-05</v>
       </c>
       <c r="AE10" t="n">
-        <v>-3.664265669874047e-06</v>
+        <v>-4.763365750305478e-05</v>
       </c>
       <c r="AF10" t="n">
-        <v>7.37236597418614e-05</v>
+        <v>-1.754831882644246e-05</v>
       </c>
       <c r="AG10" t="n">
-        <v>3.24313821898932e-05</v>
+        <v>5.322401685014712e-05</v>
       </c>
       <c r="AH10" t="n">
-        <v>-6.0283971876563e-05</v>
+        <v>-0.0006445950341095861</v>
       </c>
       <c r="AI10" t="n">
-        <v>4.57983784108557e-05</v>
+        <v>-0.0009917877890339274</v>
       </c>
       <c r="AJ10" t="n">
-        <v>-7.257117343298604e-05</v>
+        <v>-0.0003990007450472555</v>
       </c>
       <c r="AK10" t="n">
-        <v>7.780232546299756e-05</v>
+        <v>0.0004213896295895422</v>
       </c>
       <c r="AL10" t="n">
-        <v>-3.453775738594633e-05</v>
+        <v>0.0001223980526670682</v>
       </c>
       <c r="AM10" t="n">
-        <v>1.223931131860855e-05</v>
+        <v>-0.0005347839501926861</v>
       </c>
       <c r="AN10" t="n">
-        <v>-4.052653189961699e-05</v>
+        <v>-0.0002906075543669415</v>
       </c>
       <c r="AO10" t="n">
-        <v>5.197100213082437e-05</v>
+        <v>0.0003409657801087236</v>
       </c>
       <c r="AP10" t="n">
-        <v>-2.067277650406911e-05</v>
+        <v>6.665278783972634e-05</v>
       </c>
       <c r="AQ10" t="n">
-        <v>8.881540460746051e-07</v>
+        <v>-0.0005087126296724283</v>
       </c>
       <c r="AR10" t="n">
-        <v>-1.934990446598109e-05</v>
+        <v>-0.0001931702640664422</v>
       </c>
       <c r="AS10" t="n">
-        <v>3.178063794509458e-05</v>
+        <v>0.0004480675282011276</v>
       </c>
       <c r="AT10" t="n">
-        <v>-1.287589334332308e-05</v>
+        <v>0.0001428949139659717</v>
       </c>
       <c r="AU10" t="n">
-        <v>-2.908646027652812e-06</v>
+        <v>-0.0004978622469339363</v>
       </c>
       <c r="AV10" t="n">
-        <v>-8.215139704254001e-06</v>
+        <v>-0.0002056882089594981</v>
       </c>
       <c r="AW10" t="n">
-        <v>1.93043816781864e-05</v>
+        <v>0.0004563483158026895</v>
       </c>
       <c r="AX10" t="n">
-        <v>-0.0003221546823674668</v>
+        <v>0.0004214351822502868</v>
       </c>
       <c r="AY10" t="n">
-        <v>8.038390210105508e-05</v>
+        <v>-1.547978295835814e-05</v>
       </c>
       <c r="AZ10" t="n">
-        <v>8.531987829242041e-05</v>
+        <v>-0.0001443716367741423</v>
       </c>
       <c r="BA10" t="n">
-        <v>-9.750266313907187e-06</v>
+        <v>-2.638259381156993e-07</v>
       </c>
       <c r="BB10" t="n">
-        <v>-0.0001794106152369146</v>
+        <v>0.0003422853571893834</v>
       </c>
       <c r="BC10" t="n">
-        <v>7.929059931092063e-05</v>
+        <v>-5.335058938248978e-06</v>
       </c>
       <c r="BD10" t="n">
-        <v>7.1633850620545e-05</v>
+        <v>-0.000212150833987332</v>
       </c>
       <c r="BE10" t="n">
-        <v>-2.559289378101197e-05</v>
+        <v>-7.735295122618524e-06</v>
       </c>
       <c r="BF10" t="n">
-        <v>-0.0001056178867479846</v>
+        <v>0.0003027560045743789</v>
       </c>
       <c r="BG10" t="n">
-        <v>6.449376501011359e-05</v>
+        <v>2.742089693508704e-06</v>
       </c>
       <c r="BH10" t="n">
-        <v>4.891737162871557e-05</v>
+        <v>-0.0002440734339955185</v>
       </c>
       <c r="BI10" t="n">
-        <v>-3.117065958383373e-05</v>
+        <v>-1.175711276249527e-05</v>
       </c>
       <c r="BJ10" t="n">
-        <v>-6.190050581578163e-05</v>
+        <v>0.0002877287258341529</v>
       </c>
       <c r="BK10" t="n">
-        <v>4.989416596359252e-05</v>
+        <v>1.028771701435968e-05</v>
       </c>
       <c r="BL10" t="n">
-        <v>3.042066366208748e-05</v>
+        <v>-0.0002618345269249247</v>
       </c>
       <c r="BM10" t="n">
-        <v>-2.969763515772696e-05</v>
+        <v>-1.735702302297607e-05</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.01124494479166272</v>
+        <v>-0.006817454136490148</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.001520653198364417</v>
+        <v>-0.002824349490402249</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00266885419042949</v>
+        <v>0.001908746294458336</v>
       </c>
       <c r="E11" t="n">
-        <v>0.001348636604942609</v>
+        <v>0.0009183449647471652</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0005595281414116825</v>
+        <v>0.00141196092540656</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.0002341283208079955</v>
+        <v>-0.0004708797051527248</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.0003985426764480988</v>
+        <v>-0.0007148733136847689</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.0001005081014103814</v>
+        <v>-0.0009767874470779463</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.000101081676487103</v>
+        <v>0.000503078560413692</v>
       </c>
       <c r="K11" t="n">
-        <v>3.131156799055212e-05</v>
+        <v>0.0001313498933376699</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0001862408915076848</v>
+        <v>0.0005337048892192508</v>
       </c>
       <c r="M11" t="n">
-        <v>7.414954970476478e-05</v>
+        <v>-0.000473385020645305</v>
       </c>
       <c r="N11" t="n">
-        <v>-0.0001538275181453616</v>
+        <v>0.0002195642953954438</v>
       </c>
       <c r="O11" t="n">
-        <v>-7.631298914762942e-05</v>
+        <v>-0.0003286676193286278</v>
       </c>
       <c r="P11" t="n">
-        <v>0.0001182547388272683</v>
+        <v>0.0002696613894595519</v>
       </c>
       <c r="Q11" t="n">
-        <v>6.724241467487257e-05</v>
+        <v>-0.0003676975644150233</v>
       </c>
       <c r="R11" t="n">
-        <v>4.827618317432849e-05</v>
+        <v>0.001216055286032424</v>
       </c>
       <c r="S11" t="n">
-        <v>-9.583178369320356e-06</v>
+        <v>-0.0002795745100847273</v>
       </c>
       <c r="T11" t="n">
-        <v>6.267415724130409e-05</v>
+        <v>-0.0005691126335926916</v>
       </c>
       <c r="U11" t="n">
-        <v>-0.0001243332437738888</v>
+        <v>-0.0005830951630117643</v>
       </c>
       <c r="V11" t="n">
-        <v>1.185154139864934e-05</v>
+        <v>0.0001573277791492809</v>
       </c>
       <c r="W11" t="n">
-        <v>6.296709643398501e-05</v>
+        <v>0.0002197927588826258</v>
       </c>
       <c r="X11" t="n">
-        <v>3.647762769452132e-05</v>
+        <v>0.0002600650604791017</v>
       </c>
       <c r="Y11" t="n">
-        <v>-9.414465817093889e-05</v>
+        <v>-0.0003018505284590701</v>
       </c>
       <c r="Z11" t="n">
-        <v>-3.694385046253209e-06</v>
+        <v>8.963026103253453e-05</v>
       </c>
       <c r="AA11" t="n">
-        <v>6.61388418182574e-05</v>
+        <v>-5.266494003405934e-05</v>
       </c>
       <c r="AB11" t="n">
-        <v>2.225588746447834e-05</v>
+        <v>6.847123617284079e-05</v>
       </c>
       <c r="AC11" t="n">
-        <v>-8.118656124590128e-05</v>
+        <v>-0.000240644385097675</v>
       </c>
       <c r="AD11" t="n">
-        <v>-7.600354744077047e-06</v>
+        <v>0.0002165385274900791</v>
       </c>
       <c r="AE11" t="n">
-        <v>6.902513163157527e-05</v>
+        <v>2.065604119064575e-05</v>
       </c>
       <c r="AF11" t="n">
-        <v>1.532772206112763e-05</v>
+        <v>5.76281716373613e-05</v>
       </c>
       <c r="AG11" t="n">
-        <v>-7.445180756781202e-05</v>
+        <v>-0.0002792229617869397</v>
       </c>
       <c r="AH11" t="n">
-        <v>4.014843455820409e-05</v>
+        <v>-0.001868834067770949</v>
       </c>
       <c r="AI11" t="n">
-        <v>-0.001207381575236411</v>
+        <v>0.00116936493897521</v>
       </c>
       <c r="AJ11" t="n">
-        <v>-0.0005087488712532211</v>
+        <v>-0.0009875989338892117</v>
       </c>
       <c r="AK11" t="n">
-        <v>0.0003502992033153338</v>
+        <v>0.0006297560445297976</v>
       </c>
       <c r="AL11" t="n">
-        <v>7.040955581303119e-05</v>
+        <v>-0.001740714892398925</v>
       </c>
       <c r="AM11" t="n">
-        <v>-0.0006387329502917993</v>
+        <v>0.001521490567209997</v>
       </c>
       <c r="AN11" t="n">
-        <v>-0.0001451339775537079</v>
+        <v>-0.0003756569660115169</v>
       </c>
       <c r="AO11" t="n">
-        <v>0.0004622386568182677</v>
+        <v>0.0006658859921988707</v>
       </c>
       <c r="AP11" t="n">
-        <v>7.964270109385136e-05</v>
+        <v>-0.001765616011150358</v>
       </c>
       <c r="AQ11" t="n">
-        <v>-0.0005700032314892271</v>
+        <v>0.001396342869298769</v>
       </c>
       <c r="AR11" t="n">
-        <v>-0.0001086438667279979</v>
+        <v>-0.0004281498384506311</v>
       </c>
       <c r="AS11" t="n">
-        <v>0.0004961741849321868</v>
+        <v>0.000690976793022293</v>
       </c>
       <c r="AT11" t="n">
-        <v>9.11568422481247e-05</v>
+        <v>-0.001603205660755752</v>
       </c>
       <c r="AU11" t="n">
-        <v>-0.0005175015664254261</v>
+        <v>0.001383436954469312</v>
       </c>
       <c r="AV11" t="n">
-        <v>-8.676562118368263e-05</v>
+        <v>-0.0004561865280287833</v>
       </c>
       <c r="AW11" t="n">
-        <v>0.0004855017759391453</v>
+        <v>0.0006279972710057978</v>
       </c>
       <c r="AX11" t="n">
-        <v>-0.000512202851873453</v>
+        <v>-0.001481409670242136</v>
       </c>
       <c r="AY11" t="n">
-        <v>5.072483337081829e-05</v>
+        <v>0.0008190640786055996</v>
       </c>
       <c r="AZ11" t="n">
-        <v>0.0001908454348889969</v>
+        <v>0.0004753683442458637</v>
       </c>
       <c r="BA11" t="n">
-        <v>4.372283268432603e-06</v>
+        <v>1.469140024617399e-05</v>
       </c>
       <c r="BB11" t="n">
-        <v>-0.0003746552979910644</v>
+        <v>-0.001325822076303825</v>
       </c>
       <c r="BC11" t="n">
-        <v>4.631743467543516e-05</v>
+        <v>0.0007759242408129056</v>
       </c>
       <c r="BD11" t="n">
-        <v>0.0002507635651891117</v>
+        <v>0.0003994069690658975</v>
       </c>
       <c r="BE11" t="n">
-        <v>-1.108118314065868e-05</v>
+        <v>5.369274018256173e-05</v>
       </c>
       <c r="BF11" t="n">
-        <v>-0.0003147467971448381</v>
+        <v>-0.001201982913856476</v>
       </c>
       <c r="BG11" t="n">
-        <v>4.169023549593001e-05</v>
+        <v>0.0007877262001044842</v>
       </c>
       <c r="BH11" t="n">
-        <v>0.000263064741423747</v>
+        <v>0.000353730878009706</v>
       </c>
       <c r="BI11" t="n">
-        <v>-2.383519513086031e-05</v>
+        <v>1.644672141746335e-05</v>
       </c>
       <c r="BJ11" t="n">
-        <v>-0.00028377946705019</v>
+        <v>-0.00113987776187163</v>
       </c>
       <c r="BK11" t="n">
-        <v>4.010279071250731e-05</v>
+        <v>0.0007840810099507797</v>
       </c>
       <c r="BL11" t="n">
-        <v>0.0002593014128646509</v>
+        <v>0.0003212902493106685</v>
       </c>
       <c r="BM11" t="n">
-        <v>-3.238152266751837e-05</v>
+        <v>3.116573100228982e-06</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>NewZealand</t>
+          <t>Lithuania</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.001844770950923809</v>
+        <v>-0.01124494479166272</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.0005252721056858477</v>
+        <v>-0.001520653198364417</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0003409218328701549</v>
+        <v>0.00266885419042949</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0002330757610616912</v>
+        <v>0.001348636604942609</v>
       </c>
       <c r="F12" t="n">
-        <v>-1.724212818082704e-05</v>
+        <v>0.0005595281414116825</v>
       </c>
       <c r="G12" t="n">
-        <v>-6.382315009443081e-05</v>
+        <v>-0.0002341283208079955</v>
       </c>
       <c r="H12" t="n">
-        <v>-1.532173342893182e-05</v>
+        <v>-0.0003985426764480988</v>
       </c>
       <c r="I12" t="n">
-        <v>1.13453294446733e-05</v>
+        <v>-0.0001005081014103814</v>
       </c>
       <c r="J12" t="n">
-        <v>7.445738882396754e-06</v>
+        <v>-0.000101081676487103</v>
       </c>
       <c r="K12" t="n">
-        <v>-5.426226723386777e-07</v>
+        <v>3.131156799055212e-05</v>
       </c>
       <c r="L12" t="n">
-        <v>-2.068992621807933e-06</v>
+        <v>0.0001862408915076848</v>
       </c>
       <c r="M12" t="n">
-        <v>-5.12732290966494e-07</v>
+        <v>7.414954970476478e-05</v>
       </c>
       <c r="N12" t="n">
-        <v>3.671196111080049e-07</v>
+        <v>-0.0001538275181453616</v>
       </c>
       <c r="O12" t="n">
-        <v>2.463042958362792e-07</v>
+        <v>-7.631298914762942e-05</v>
       </c>
       <c r="P12" t="n">
-        <v>-1.641541287521996e-08</v>
+        <v>0.0001182547388272683</v>
       </c>
       <c r="Q12" t="n">
-        <v>-6.804469817288168e-08</v>
+        <v>6.724241467487257e-05</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0001133302537582249</v>
+        <v>4.827618317432849e-05</v>
       </c>
       <c r="S12" t="n">
-        <v>6.176850202814514e-05</v>
+        <v>-9.583178369320356e-06</v>
       </c>
       <c r="T12" t="n">
-        <v>7.775046083533069e-05</v>
+        <v>6.267415724130409e-05</v>
       </c>
       <c r="U12" t="n">
-        <v>-3.84137821911569e-06</v>
+        <v>-0.0001243332437738888</v>
       </c>
       <c r="V12" t="n">
-        <v>-2.355009655523186e-05</v>
+        <v>1.185154139864934e-05</v>
       </c>
       <c r="W12" t="n">
-        <v>-4.887157153101229e-06</v>
+        <v>6.296709643398501e-05</v>
       </c>
       <c r="X12" t="n">
-        <v>4.661912561255115e-06</v>
+        <v>3.647762769452132e-05</v>
       </c>
       <c r="Y12" t="n">
-        <v>2.531742451738756e-06</v>
+        <v>-9.414465817093889e-05</v>
       </c>
       <c r="Z12" t="n">
-        <v>-4.050999478932331e-07</v>
+        <v>-3.694385046253209e-06</v>
       </c>
       <c r="AA12" t="n">
-        <v>-7.530984410373949e-07</v>
+        <v>6.61388418182574e-05</v>
       </c>
       <c r="AB12" t="n">
-        <v>-1.330804277500917e-07</v>
+        <v>2.225588746447834e-05</v>
       </c>
       <c r="AC12" t="n">
-        <v>1.482424048777899e-07</v>
+        <v>-8.118656124590128e-05</v>
       </c>
       <c r="AD12" t="n">
-        <v>8.063886795178541e-08</v>
+        <v>-7.600354744077047e-06</v>
       </c>
       <c r="AE12" t="n">
-        <v>-1.229671792347337e-08</v>
+        <v>6.902513163157527e-05</v>
       </c>
       <c r="AF12" t="n">
-        <v>-2.447248789122826e-08</v>
+        <v>1.532772206112763e-05</v>
       </c>
       <c r="AG12" t="n">
-        <v>-4.56544120506658e-09</v>
+        <v>-7.445180756781202e-05</v>
       </c>
       <c r="AH12" t="n">
-        <v>-5.667059030262301e-05</v>
+        <v>4.014843455820409e-05</v>
       </c>
       <c r="AI12" t="n">
-        <v>-7.700705123095396e-05</v>
+        <v>-0.001207381575236411</v>
       </c>
       <c r="AJ12" t="n">
-        <v>9.594216730967735e-06</v>
+        <v>-0.0005087488712532211</v>
       </c>
       <c r="AK12" t="n">
-        <v>2.803950025104307e-05</v>
+        <v>0.0003502992033153338</v>
       </c>
       <c r="AL12" t="n">
-        <v>3.905105476336399e-06</v>
+        <v>7.040955581303119e-05</v>
       </c>
       <c r="AM12" t="n">
-        <v>-6.377551473475951e-06</v>
+        <v>-0.0006387329502917993</v>
       </c>
       <c r="AN12" t="n">
-        <v>-2.7022878622261e-06</v>
+        <v>-0.0001451339775537079</v>
       </c>
       <c r="AO12" t="n">
-        <v>8.11315604061255e-07</v>
+        <v>0.0004622386568182677</v>
       </c>
       <c r="AP12" t="n">
-        <v>9.0990211657568e-07</v>
+        <v>7.964270109385136e-05</v>
       </c>
       <c r="AQ12" t="n">
-        <v>7.704588312011679e-08</v>
+        <v>-0.0005700032314892271</v>
       </c>
       <c r="AR12" t="n">
-        <v>-2.041939543765025e-07</v>
+        <v>-0.0001086438667279979</v>
       </c>
       <c r="AS12" t="n">
-        <v>-8.38222479122803e-08</v>
+        <v>0.0004961741849321868</v>
       </c>
       <c r="AT12" t="n">
-        <v>2.539247819533712e-08</v>
+        <v>9.11568422481247e-05</v>
       </c>
       <c r="AU12" t="n">
-        <v>2.93979280798473e-08</v>
+        <v>-0.0005175015664254261</v>
       </c>
       <c r="AV12" t="n">
-        <v>2.788849651512442e-09</v>
+        <v>-8.676562118368263e-05</v>
       </c>
       <c r="AW12" t="n">
-        <v>-6.63498330535317e-09</v>
+        <v>0.0004855017759391453</v>
       </c>
       <c r="AX12" t="n">
-        <v>0.0001211065616595247</v>
+        <v>-0.000512202851873453</v>
       </c>
       <c r="AY12" t="n">
-        <v>-5.644049836517429e-06</v>
+        <v>5.072483337081829e-05</v>
       </c>
       <c r="AZ12" t="n">
-        <v>-5.596391993309508e-06</v>
+        <v>0.0001908454348889969</v>
       </c>
       <c r="BA12" t="n">
-        <v>2.877367434362951e-06</v>
+        <v>4.372283268432603e-06</v>
       </c>
       <c r="BB12" t="n">
-        <v>-8.421779942545265e-07</v>
+        <v>-0.0003746552979910644</v>
       </c>
       <c r="BC12" t="n">
-        <v>-1.161251283345174e-06</v>
+        <v>4.631743467543516e-05</v>
       </c>
       <c r="BD12" t="n">
-        <v>2.097624600738905e-07</v>
+        <v>0.0002507635651891117</v>
       </c>
       <c r="BE12" t="n">
-        <v>3.587253349032454e-07</v>
+        <v>-1.108118314065868e-05</v>
       </c>
       <c r="BF12" t="n">
-        <v>1.967952983374167e-08</v>
+        <v>-0.0003147467971448381</v>
       </c>
       <c r="BG12" t="n">
-        <v>-8.265640519933747e-08</v>
+        <v>4.169023549593001e-05</v>
       </c>
       <c r="BH12" t="n">
-        <v>-2.67910906370393e-08</v>
+        <v>0.000263064741423747</v>
       </c>
       <c r="BI12" t="n">
-        <v>1.214086002229205e-08</v>
+        <v>-2.383519513086031e-05</v>
       </c>
       <c r="BJ12" t="n">
-        <v>1.022182575146466e-08</v>
+        <v>-0.00028377946705019</v>
       </c>
       <c r="BK12" t="n">
-        <v>1.948365182048541e-10</v>
+        <v>4.010279071250731e-05</v>
       </c>
       <c r="BL12" t="n">
-        <v>-2.506111877177766e-09</v>
+        <v>0.0002593014128646509</v>
       </c>
       <c r="BM12" t="n">
-        <v>-8.481686077771498e-10</v>
+        <v>-3.238152266751837e-05</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3.350854589930979e-16</v>
+        <v>-0.01340195179942198</v>
       </c>
       <c r="C13" t="n">
-        <v>8.57641546884664e-17</v>
+        <v>-0.00215910423311057</v>
       </c>
       <c r="D13" t="n">
-        <v>5.827727981547471e-18</v>
+        <v>0.004320808062186363</v>
       </c>
       <c r="E13" t="n">
-        <v>-4.620780776611795e-17</v>
+        <v>0.001239627817110118</v>
       </c>
       <c r="F13" t="n">
-        <v>2.751924501713556e-19</v>
+        <v>3.44205137102013e-05</v>
       </c>
       <c r="G13" t="n">
-        <v>1.813586247263823e-17</v>
+        <v>0.0008204165520472403</v>
       </c>
       <c r="H13" t="n">
-        <v>1.389945995986441e-17</v>
+        <v>-0.0002700300836826422</v>
       </c>
       <c r="I13" t="n">
-        <v>3.230587888701884e-18</v>
+        <v>-0.0005316160576060891</v>
       </c>
       <c r="J13" t="n">
-        <v>-1.134100148960023e-18</v>
+        <v>-0.0006767830446146051</v>
       </c>
       <c r="K13" t="n">
-        <v>5.378990089184732e-18</v>
+        <v>0.0003289585658482285</v>
       </c>
       <c r="L13" t="n">
-        <v>1.72624826750084e-18</v>
+        <v>0.0003543857914316529</v>
       </c>
       <c r="M13" t="n">
-        <v>1.975858643188285e-18</v>
+        <v>0.0001741995960301874</v>
       </c>
       <c r="N13" t="n">
-        <v>-1.357950914947365e-18</v>
+        <v>-0.0003995763720469457</v>
       </c>
       <c r="O13" t="n">
-        <v>4.11677611147856e-18</v>
+        <v>0.0001072739186662811</v>
       </c>
       <c r="P13" t="n">
-        <v>3.061998965646183e-19</v>
+        <v>4.241800913070983e-05</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.25107388871035e-18</v>
+        <v>9.729781752616009e-05</v>
       </c>
       <c r="R13" t="n">
-        <v>-1.822089403079222e-16</v>
+        <v>0.0001142886858605279</v>
       </c>
       <c r="S13" t="n">
-        <v>2.248126013204231e-17</v>
+        <v>-0.0002334590476133944</v>
       </c>
       <c r="T13" t="n">
-        <v>3.172965824986415e-17</v>
+        <v>-3.429228997985494e-05</v>
       </c>
       <c r="U13" t="n">
-        <v>5.096098773166992e-17</v>
+        <v>-0.0001376930675648804</v>
       </c>
       <c r="V13" t="n">
-        <v>1.272870653504502e-17</v>
+        <v>0.0005037309300786058</v>
       </c>
       <c r="W13" t="n">
-        <v>2.564443090085199e-17</v>
+        <v>-3.924766517760296e-05</v>
       </c>
       <c r="X13" t="n">
-        <v>1.033556471223158e-18</v>
+        <v>-6.958059501682217e-05</v>
       </c>
       <c r="Y13" t="n">
-        <v>5.145158816979649e-18</v>
+        <v>-0.0002091360895161582</v>
       </c>
       <c r="Z13" t="n">
-        <v>-2.674856738717085e-19</v>
+        <v>0.0002578039087886762</v>
       </c>
       <c r="AA13" t="n">
-        <v>1.908324822885671e-17</v>
+        <v>-7.380443774571235e-05</v>
       </c>
       <c r="AB13" t="n">
-        <v>2.329076783362274e-18</v>
+        <v>3.397037461428601e-05</v>
       </c>
       <c r="AC13" t="n">
-        <v>2.492987108973205e-18</v>
+        <v>-0.0001452533319372399</v>
       </c>
       <c r="AD13" t="n">
-        <v>-6.132034781310492e-18</v>
+        <v>0.0001766890213592016</v>
       </c>
       <c r="AE13" t="n">
-        <v>1.148830834412567e-17</v>
+        <v>-7.458922031190261e-05</v>
       </c>
       <c r="AF13" t="n">
-        <v>5.077701363974743e-19</v>
+        <v>5.275247763382585e-05</v>
       </c>
       <c r="AG13" t="n">
-        <v>2.983311323903732e-18</v>
+        <v>-0.0001221796534716068</v>
       </c>
       <c r="AH13" t="n">
-        <v>5.200162940398799e-17</v>
+        <v>-6.580829577023781e-05</v>
       </c>
       <c r="AI13" t="n">
-        <v>-5.933756723342589e-18</v>
+        <v>-0.0007363228526325701</v>
       </c>
       <c r="AJ13" t="n">
-        <v>2.257094138429085e-18</v>
+        <v>-0.000196575159803734</v>
       </c>
       <c r="AK13" t="n">
-        <v>-1.284721676988606e-17</v>
+        <v>0.0001981667385002265</v>
       </c>
       <c r="AL13" t="n">
-        <v>5.150275074523298e-17</v>
+        <v>0.000530052428104713</v>
       </c>
       <c r="AM13" t="n">
-        <v>-5.080107895749152e-18</v>
+        <v>-0.000246549695441277</v>
       </c>
       <c r="AN13" t="n">
-        <v>2.909706666169467e-18</v>
+        <v>-0.0001442107370915589</v>
       </c>
       <c r="AO13" t="n">
-        <v>-2.434329301952605e-17</v>
+        <v>-5.738948063004866e-05</v>
       </c>
       <c r="AP13" t="n">
-        <v>3.621117281073781e-17</v>
+        <v>0.0002601067252402717</v>
       </c>
       <c r="AQ13" t="n">
-        <v>-5.154730422133643e-18</v>
+        <v>-0.0001642485840309623</v>
       </c>
       <c r="AR13" t="n">
-        <v>7.767441178062811e-18</v>
+        <v>-1.395338895941474e-05</v>
       </c>
       <c r="AS13" t="n">
-        <v>-2.562814723190435e-17</v>
+        <v>-5.23110844716494e-05</v>
       </c>
       <c r="AT13" t="n">
-        <v>2.619991780871358e-17</v>
+        <v>0.0001858774959933383</v>
       </c>
       <c r="AU13" t="n">
-        <v>-6.18198398159948e-18</v>
+        <v>-0.0001143103217580227</v>
       </c>
       <c r="AV13" t="n">
-        <v>1.124395265947914e-17</v>
+        <v>1.435799618851657e-05</v>
       </c>
       <c r="AW13" t="n">
-        <v>-2.399992184899628e-17</v>
+        <v>-7.011151867722117e-05</v>
       </c>
       <c r="AX13" t="n">
-        <v>2.254855575794018e-16</v>
+        <v>-0.0004264667967940048</v>
       </c>
       <c r="AY13" t="n">
-        <v>-2.016881280613513e-17</v>
+        <v>5.77292331510995e-05</v>
       </c>
       <c r="AZ13" t="n">
-        <v>-1.272363162689549e-17</v>
+        <v>-1.837911910455632e-05</v>
       </c>
       <c r="BA13" t="n">
-        <v>-6.024822096665147e-17</v>
+        <v>0.0001000381288411034</v>
       </c>
       <c r="BB13" t="n">
-        <v>1.458756263977994e-16</v>
+        <v>-0.0002178869855760796</v>
       </c>
       <c r="BC13" t="n">
-        <v>-1.770326062225913e-17</v>
+        <v>8.627766153731088e-05</v>
       </c>
       <c r="BD13" t="n">
-        <v>4.221729037705183e-18</v>
+        <v>-3.784954780883978e-05</v>
       </c>
       <c r="BE13" t="n">
-        <v>-7.518066439088609e-17</v>
+        <v>9.977981017687423e-05</v>
       </c>
       <c r="BF13" t="n">
-        <v>1.042780418148685e-16</v>
+        <v>-0.0001485039658908128</v>
       </c>
       <c r="BG13" t="n">
-        <v>-1.670626415373184e-17</v>
+        <v>7.575048552442566e-05</v>
       </c>
       <c r="BH13" t="n">
-        <v>1.95288132004966e-17</v>
+        <v>-4.925874690211417e-05</v>
       </c>
       <c r="BI13" t="n">
-        <v>-7.677835574398287e-17</v>
+        <v>9.030254526872171e-05</v>
       </c>
       <c r="BJ13" t="n">
-        <v>7.650608026584854e-17</v>
+        <v>-0.0001054289674749679</v>
       </c>
       <c r="BK13" t="n">
-        <v>-1.800179381524212e-17</v>
+        <v>6.630138853474988e-05</v>
       </c>
       <c r="BL13" t="n">
-        <v>3.12195959161396e-17</v>
+        <v>-5.373156436809087e-05</v>
       </c>
       <c r="BM13" t="n">
-        <v>-7.132233385823511e-17</v>
+        <v>7.582441429277511e-05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>SouthAfrica</t>
+          <t>NewZealand</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0004886071866749847</v>
+        <v>-0.001844770950923809</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0001283848457481581</v>
+        <v>-0.0005252721056858477</v>
       </c>
       <c r="D14" t="n">
-        <v>3.406586550309955e-05</v>
+        <v>0.0003409218328701549</v>
       </c>
       <c r="E14" t="n">
-        <v>9.207381014673889e-06</v>
+        <v>0.0002330757610616912</v>
       </c>
       <c r="F14" t="n">
-        <v>2.573085639575122e-06</v>
+        <v>-1.724212818082704e-05</v>
       </c>
       <c r="G14" t="n">
-        <v>7.607252799301883e-07</v>
+        <v>-6.382315009443081e-05</v>
       </c>
       <c r="H14" t="n">
-        <v>2.447647361593976e-07</v>
+        <v>-1.532173342893182e-05</v>
       </c>
       <c r="I14" t="n">
-        <v>8.770279430492774e-08</v>
+        <v>1.13453294446733e-05</v>
       </c>
       <c r="J14" t="n">
-        <v>3.513101090230767e-08</v>
+        <v>7.445738882396754e-06</v>
       </c>
       <c r="K14" t="n">
-        <v>1.545034370378417e-08</v>
+        <v>-5.426226723386777e-07</v>
       </c>
       <c r="L14" t="n">
-        <v>7.253264729847675e-09</v>
+        <v>-2.068992621807933e-06</v>
       </c>
       <c r="M14" t="n">
-        <v>3.543940979762612e-09</v>
+        <v>-5.12732290966494e-07</v>
       </c>
       <c r="N14" t="n">
-        <v>1.770973442444183e-09</v>
+        <v>3.671196111080049e-07</v>
       </c>
       <c r="O14" t="n">
-        <v>8.957339156397494e-10</v>
+        <v>2.463042958362792e-07</v>
       </c>
       <c r="P14" t="n">
-        <v>4.559147783215999e-10</v>
+        <v>-1.641541287521996e-08</v>
       </c>
       <c r="Q14" t="n">
-        <v>2.328082859408469e-10</v>
+        <v>-6.804469817288168e-08</v>
       </c>
       <c r="R14" t="n">
-        <v>2.496327006937845e-06</v>
+        <v>-0.0001133302537582249</v>
       </c>
       <c r="S14" t="n">
-        <v>-5.682331730421668e-07</v>
+        <v>6.176850202814514e-05</v>
       </c>
       <c r="T14" t="n">
-        <v>-7.715019618252645e-07</v>
+        <v>7.775046083533069e-05</v>
       </c>
       <c r="U14" t="n">
-        <v>-5.202035569562496e-07</v>
+        <v>-3.84137821911569e-06</v>
       </c>
       <c r="V14" t="n">
-        <v>-2.990171735677575e-07</v>
+        <v>-2.355009655523186e-05</v>
       </c>
       <c r="W14" t="n">
-        <v>-1.616533375374161e-07</v>
+        <v>-4.887157153101229e-06</v>
       </c>
       <c r="X14" t="n">
-        <v>-8.502246912397576e-08</v>
+        <v>4.661912561255115e-06</v>
       </c>
       <c r="Y14" t="n">
-        <v>-4.413399405905112e-08</v>
+        <v>2.531742451738756e-06</v>
       </c>
       <c r="Z14" t="n">
-        <v>-2.276139987217152e-08</v>
+        <v>-4.050999478932331e-07</v>
       </c>
       <c r="AA14" t="n">
-        <v>-1.170085283787316e-08</v>
+        <v>-7.530984410373949e-07</v>
       </c>
       <c r="AB14" t="n">
-        <v>-6.005195791404332e-09</v>
+        <v>-1.330804277500917e-07</v>
       </c>
       <c r="AC14" t="n">
-        <v>-3.079487157512642e-09</v>
+        <v>1.482424048777899e-07</v>
       </c>
       <c r="AD14" t="n">
-        <v>-1.578512625787981e-09</v>
+        <v>8.063886795178541e-08</v>
       </c>
       <c r="AE14" t="n">
-        <v>-8.089574243695408e-10</v>
+        <v>-1.229671792347337e-08</v>
       </c>
       <c r="AF14" t="n">
-        <v>-4.14530578592058e-10</v>
+        <v>-2.447248789122826e-08</v>
       </c>
       <c r="AG14" t="n">
-        <v>-2.124045354437271e-10</v>
+        <v>-4.56544120506658e-09</v>
       </c>
       <c r="AH14" t="n">
-        <v>9.287828073714382e-06</v>
+        <v>-5.667059030262301e-05</v>
       </c>
       <c r="AI14" t="n">
-        <v>1.406487635531341e-05</v>
+        <v>-7.700705123095396e-05</v>
       </c>
       <c r="AJ14" t="n">
-        <v>9.626318550134779e-06</v>
+        <v>9.594216730967735e-06</v>
       </c>
       <c r="AK14" t="n">
-        <v>5.561490172935452e-06</v>
+        <v>2.803950025104307e-05</v>
       </c>
       <c r="AL14" t="n">
-        <v>3.013165776322726e-06</v>
+        <v>3.905105476336399e-06</v>
       </c>
       <c r="AM14" t="n">
-        <v>1.586402440051808e-06</v>
+        <v>-6.377551473475951e-06</v>
       </c>
       <c r="AN14" t="n">
-        <v>8.238878273427711e-07</v>
+        <v>-2.7022878622261e-06</v>
       </c>
       <c r="AO14" t="n">
-        <v>4.25011697065221e-07</v>
+        <v>8.11315604061255e-07</v>
       </c>
       <c r="AP14" t="n">
-        <v>2.185109592522193e-07</v>
+        <v>9.0990211657568e-07</v>
       </c>
       <c r="AQ14" t="n">
-        <v>1.121527792101218e-07</v>
+        <v>7.704588312011679e-08</v>
       </c>
       <c r="AR14" t="n">
-        <v>5.751419105251429e-08</v>
+        <v>-2.041939543765025e-07</v>
       </c>
       <c r="AS14" t="n">
-        <v>2.9481640605523e-08</v>
+        <v>-8.38222479122803e-08</v>
       </c>
       <c r="AT14" t="n">
-        <v>1.510889793858584e-08</v>
+        <v>2.539247819533712e-08</v>
       </c>
       <c r="AU14" t="n">
-        <v>7.742219648934273e-09</v>
+        <v>2.93979280798473e-08</v>
       </c>
       <c r="AV14" t="n">
-        <v>3.967104234113454e-09</v>
+        <v>2.788849651512442e-09</v>
       </c>
       <c r="AW14" t="n">
-        <v>2.032681165518262e-09</v>
+        <v>-6.63498330535317e-09</v>
       </c>
       <c r="AX14" t="n">
-        <v>-4.283023336123716e-05</v>
+        <v>0.0001211065616595247</v>
       </c>
       <c r="AY14" t="n">
-        <v>-2.180392914491935e-05</v>
+        <v>-5.644049836517429e-06</v>
       </c>
       <c r="AZ14" t="n">
-        <v>-1.113500356050127e-05</v>
+        <v>-5.596391993309508e-06</v>
       </c>
       <c r="BA14" t="n">
-        <v>-5.695699050045989e-06</v>
+        <v>2.877367434362951e-06</v>
       </c>
       <c r="BB14" t="n">
-        <v>-2.91582092387228e-06</v>
+        <v>-8.421779942545265e-07</v>
       </c>
       <c r="BC14" t="n">
-        <v>-1.493331623091798e-06</v>
+        <v>-1.161251283345174e-06</v>
       </c>
       <c r="BD14" t="n">
-        <v>-7.649691648059772e-07</v>
+        <v>2.097624600738905e-07</v>
       </c>
       <c r="BE14" t="n">
-        <v>-3.919028667985148e-07</v>
+        <v>3.587253349032454e-07</v>
       </c>
       <c r="BF14" t="n">
-        <v>-2.007875270724512e-07</v>
+        <v>1.967952983374167e-08</v>
       </c>
       <c r="BG14" t="n">
-        <v>-1.028743470060837e-07</v>
+        <v>-8.265640519933747e-08</v>
       </c>
       <c r="BH14" t="n">
-        <v>-5.270885454377946e-08</v>
+        <v>-2.67910906370393e-08</v>
       </c>
       <c r="BI14" t="n">
-        <v>-2.700618101856199e-08</v>
+        <v>1.214086002229205e-08</v>
       </c>
       <c r="BJ14" t="n">
-        <v>-1.383707670296621e-08</v>
+        <v>1.022182575146466e-08</v>
       </c>
       <c r="BK14" t="n">
-        <v>-7.089674938789731e-09</v>
+        <v>1.948365182048541e-10</v>
       </c>
       <c r="BL14" t="n">
-        <v>-3.632525775383655e-09</v>
+        <v>-2.506111877177766e-09</v>
       </c>
       <c r="BM14" t="n">
-        <v>-1.861192493354593e-09</v>
+        <v>-8.481686077771498e-10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.002684837924965605</v>
+        <v>3.350854589930979e-16</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.001030210162049437</v>
+        <v>8.57641546884664e-17</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0005409276678340413</v>
+        <v>5.827727981547471e-18</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0007093285178104128</v>
+        <v>-4.620780776611795e-17</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0006818069730132979</v>
+        <v>2.751924501713556e-19</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.0004703228548317074</v>
+        <v>1.813586247263823e-17</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.000745735711351515</v>
+        <v>1.389945995986441e-17</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.0005223794993428616</v>
+        <v>3.230587888701884e-18</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0003737394419430133</v>
+        <v>-1.134100148960023e-18</v>
       </c>
       <c r="K15" t="n">
-        <v>0.0003169856492798228</v>
+        <v>5.378990089184732e-18</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0001086798641678745</v>
+        <v>1.72624826750084e-18</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.0003199297818909044</v>
+        <v>1.975858643188285e-18</v>
       </c>
       <c r="N15" t="n">
-        <v>-5.124044986039787e-05</v>
+        <v>-1.357950914947365e-18</v>
       </c>
       <c r="O15" t="n">
-        <v>-0.0001103777368566666</v>
+        <v>4.11677611147856e-18</v>
       </c>
       <c r="P15" t="n">
-        <v>5.035627457225896e-05</v>
+        <v>3.061998965646183e-19</v>
       </c>
       <c r="Q15" t="n">
-        <v>-4.115054699897561e-05</v>
+        <v>1.25107388871035e-18</v>
       </c>
       <c r="R15" t="n">
-        <v>-0.0005773481470784791</v>
+        <v>-1.822089403079222e-16</v>
       </c>
       <c r="S15" t="n">
-        <v>0.000113098764525269</v>
+        <v>2.248126013204231e-17</v>
       </c>
       <c r="T15" t="n">
-        <v>0.0002769120813254084</v>
+        <v>3.172965824986415e-17</v>
       </c>
       <c r="U15" t="n">
-        <v>0.0002176618141737224</v>
+        <v>5.096098773166992e-17</v>
       </c>
       <c r="V15" t="n">
-        <v>-8.099160497194758e-05</v>
+        <v>1.272870653504502e-17</v>
       </c>
       <c r="W15" t="n">
-        <v>-3.651465845362142e-05</v>
+        <v>2.564443090085199e-17</v>
       </c>
       <c r="X15" t="n">
-        <v>-6.767072253423078e-05</v>
+        <v>1.033556471223158e-18</v>
       </c>
       <c r="Y15" t="n">
-        <v>2.859694645355165e-05</v>
+        <v>5.145158816979649e-18</v>
       </c>
       <c r="Z15" t="n">
-        <v>-2.971569119001488e-05</v>
+        <v>-2.674856738717085e-19</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.0001224798401115482</v>
+        <v>1.908324822885671e-17</v>
       </c>
       <c r="AB15" t="n">
-        <v>3.093387646007566e-05</v>
+        <v>2.329076783362274e-18</v>
       </c>
       <c r="AC15" t="n">
-        <v>-1.21726315035291e-05</v>
+        <v>2.492987108973205e-18</v>
       </c>
       <c r="AD15" t="n">
-        <v>-0.0001213941460409097</v>
+        <v>-6.132034781310492e-18</v>
       </c>
       <c r="AE15" t="n">
-        <v>4.99154435874827e-05</v>
+        <v>1.148830834412567e-17</v>
       </c>
       <c r="AF15" t="n">
-        <v>4.46961529117875e-05</v>
+        <v>5.077701363974743e-19</v>
       </c>
       <c r="AG15" t="n">
-        <v>4.151268222401253e-05</v>
+        <v>2.983311323903732e-18</v>
       </c>
       <c r="AH15" t="n">
-        <v>-0.001040146206837731</v>
+        <v>5.200162940398799e-17</v>
       </c>
       <c r="AI15" t="n">
-        <v>-0.0003562948433662743</v>
+        <v>-5.933756723342589e-18</v>
       </c>
       <c r="AJ15" t="n">
-        <v>-8.294279399410485e-05</v>
+        <v>2.257094138429085e-18</v>
       </c>
       <c r="AK15" t="n">
-        <v>0.0003811850832178101</v>
+        <v>-1.284721676988606e-17</v>
       </c>
       <c r="AL15" t="n">
-        <v>-0.0006883464522176652</v>
+        <v>5.150275074523298e-17</v>
       </c>
       <c r="AM15" t="n">
-        <v>-0.0001202505060505328</v>
+        <v>-5.080107895749152e-18</v>
       </c>
       <c r="AN15" t="n">
-        <v>-2.1750533690804e-05</v>
+        <v>2.909706666169467e-18</v>
       </c>
       <c r="AO15" t="n">
-        <v>0.0003175771916211763</v>
+        <v>-2.434329301952605e-17</v>
       </c>
       <c r="AP15" t="n">
-        <v>-0.0005744357078888721</v>
+        <v>3.621117281073781e-17</v>
       </c>
       <c r="AQ15" t="n">
-        <v>-4.030276892064774e-05</v>
+        <v>-5.154730422133643e-18</v>
       </c>
       <c r="AR15" t="n">
-        <v>6.178545324442914e-05</v>
+        <v>7.767441178062811e-18</v>
       </c>
       <c r="AS15" t="n">
-        <v>0.0003420260482801652</v>
+        <v>-2.562814723190435e-17</v>
       </c>
       <c r="AT15" t="n">
-        <v>-0.0004804002394411688</v>
+        <v>2.619991780871358e-17</v>
       </c>
       <c r="AU15" t="n">
-        <v>-4.612055924124274e-05</v>
+        <v>-6.18198398159948e-18</v>
       </c>
       <c r="AV15" t="n">
-        <v>5.169321626193795e-05</v>
+        <v>1.124395265947914e-17</v>
       </c>
       <c r="AW15" t="n">
-        <v>0.0003269560747704425</v>
+        <v>-2.399992184899628e-17</v>
       </c>
       <c r="AX15" t="n">
-        <v>0.0003797286489191955</v>
+        <v>2.254855575794018e-16</v>
       </c>
       <c r="AY15" t="n">
-        <v>-0.0001576335622625486</v>
+        <v>-2.016881280613513e-17</v>
       </c>
       <c r="AZ15" t="n">
-        <v>-5.710439578717554e-05</v>
+        <v>-1.272363162689549e-17</v>
       </c>
       <c r="BA15" t="n">
-        <v>1.754753222002368e-05</v>
+        <v>-6.024822096665147e-17</v>
       </c>
       <c r="BB15" t="n">
-        <v>0.0003211407345764097</v>
+        <v>1.458756263977994e-16</v>
       </c>
       <c r="BC15" t="n">
-        <v>-0.0001432468515826733</v>
+        <v>-1.770326062225913e-17</v>
       </c>
       <c r="BD15" t="n">
-        <v>-7.880721077708461e-05</v>
+        <v>4.221729037705183e-18</v>
       </c>
       <c r="BE15" t="n">
-        <v>-1.951433371021851e-05</v>
+        <v>-7.518066439088609e-17</v>
       </c>
       <c r="BF15" t="n">
-        <v>0.0002684943928917021</v>
+        <v>1.042780418148685e-16</v>
       </c>
       <c r="BG15" t="n">
-        <v>-0.0001205780760755438</v>
+        <v>-1.670626415373184e-17</v>
       </c>
       <c r="BH15" t="n">
-        <v>-6.7762345778202e-05</v>
+        <v>1.95288132004966e-17</v>
       </c>
       <c r="BI15" t="n">
-        <v>-2.638520243591225e-05</v>
+        <v>-7.677835574398287e-17</v>
       </c>
       <c r="BJ15" t="n">
-        <v>0.0002248632769197115</v>
+        <v>7.650608026584854e-17</v>
       </c>
       <c r="BK15" t="n">
-        <v>-0.0001096884166562223</v>
+        <v>-1.800179381524212e-17</v>
       </c>
       <c r="BL15" t="n">
-        <v>-6.300118544566062e-05</v>
+        <v>3.12195959161396e-17</v>
       </c>
       <c r="BM15" t="n">
-        <v>-2.708541722459698e-05</v>
+        <v>-7.132233385823511e-17</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.011542484778405</v>
+        <v>-0.01396051345341312</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.0027841987228592</v>
+        <v>-0.002158976928164716</v>
       </c>
       <c r="D16" t="n">
-        <v>0.002301219534904933</v>
+        <v>0.003116494644317403</v>
       </c>
       <c r="E16" t="n">
-        <v>0.002141423800213681</v>
+        <v>0.002192089939542271</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0005921746221370563</v>
+        <v>0.001487031770628142</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.0002239874546006131</v>
+        <v>-0.0005671184083243523</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.0005088516293779625</v>
+        <v>-0.001265750274180509</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.000129993192646906</v>
+        <v>-0.0004040237840816947</v>
       </c>
       <c r="J16" t="n">
-        <v>-4.701432280172318e-05</v>
+        <v>0.0002912140634641279</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0001531824945621654</v>
+        <v>0.0002589337520266327</v>
       </c>
       <c r="L16" t="n">
-        <v>3.274053524201541e-05</v>
+        <v>1.566441433938606e-05</v>
       </c>
       <c r="M16" t="n">
-        <v>4.693302467361065e-05</v>
+        <v>-4.385363863131341e-06</v>
       </c>
       <c r="N16" t="n">
-        <v>-9.884565423113951e-05</v>
+        <v>7.323272804820467e-05</v>
       </c>
       <c r="O16" t="n">
-        <v>2.750999595005686e-05</v>
+        <v>-8.87079396244289e-05</v>
       </c>
       <c r="P16" t="n">
-        <v>-9.185148750313485e-06</v>
+        <v>-0.000152722109937445</v>
       </c>
       <c r="Q16" t="n">
-        <v>4.277207210603171e-05</v>
+        <v>3.810932301609093e-05</v>
       </c>
       <c r="R16" t="n">
-        <v>2.927095768189455e-05</v>
+        <v>-0.0002139685894622191</v>
       </c>
       <c r="S16" t="n">
-        <v>-2.827039696738755e-05</v>
+        <v>8.76301931360159e-05</v>
       </c>
       <c r="T16" t="n">
-        <v>7.199866608422091e-05</v>
+        <v>0.0001226768641403904</v>
       </c>
       <c r="U16" t="n">
-        <v>-9.343602087913911e-05</v>
+        <v>8.401365196164062e-06</v>
       </c>
       <c r="V16" t="n">
-        <v>9.682269192847693e-05</v>
+        <v>-7.700029338406603e-05</v>
       </c>
       <c r="W16" t="n">
-        <v>-1.716045447717832e-05</v>
+        <v>4.260461600450783e-05</v>
       </c>
       <c r="X16" t="n">
-        <v>1.465288959506389e-05</v>
+        <v>3.739630515009481e-05</v>
       </c>
       <c r="Y16" t="n">
-        <v>-9.123390297232556e-05</v>
+        <v>-1.433675737670788e-05</v>
       </c>
       <c r="Z16" t="n">
-        <v>8.084489299605205e-05</v>
+        <v>-7.584249789264906e-05</v>
       </c>
       <c r="AA16" t="n">
-        <v>-4.154051843094286e-06</v>
+        <v>5.330356006443507e-05</v>
       </c>
       <c r="AB16" t="n">
-        <v>7.852982629980063e-06</v>
+        <v>4.33782974644208e-05</v>
       </c>
       <c r="AC16" t="n">
-        <v>-7.402035332472659e-05</v>
+        <v>-1.264869908348796e-05</v>
       </c>
       <c r="AD16" t="n">
-        <v>6.795508548853205e-05</v>
+        <v>-7.686769145436746e-05</v>
       </c>
       <c r="AE16" t="n">
-        <v>-1.682158804288142e-08</v>
+        <v>4.664935348882033e-05</v>
       </c>
       <c r="AF16" t="n">
-        <v>-6.750677671356846e-07</v>
+        <v>3.738901090664405e-05</v>
       </c>
       <c r="AG16" t="n">
-        <v>-6.043109658519211e-05</v>
+        <v>-8.765036897952209e-06</v>
       </c>
       <c r="AH16" t="n">
-        <v>0.0004655613126746067</v>
+        <v>-0.0004521498910312746</v>
       </c>
       <c r="AI16" t="n">
-        <v>-0.001077245638825984</v>
+        <v>-0.0002621452860699645</v>
       </c>
       <c r="AJ16" t="n">
-        <v>-0.0002277071482222299</v>
+        <v>8.715320815176587e-05</v>
       </c>
       <c r="AK16" t="n">
-        <v>-1.152386659833562e-05</v>
+        <v>1.026038065505312e-05</v>
       </c>
       <c r="AL16" t="n">
-        <v>0.0004122535513756173</v>
+        <v>-0.0002313720854066402</v>
       </c>
       <c r="AM16" t="n">
-        <v>-0.0003943887749922669</v>
+        <v>-5.848951006772484e-07</v>
       </c>
       <c r="AN16" t="n">
-        <v>0.0001073968974709503</v>
+        <v>0.0001723622650875499</v>
       </c>
       <c r="AO16" t="n">
-        <v>4.760599359832952e-05</v>
+        <v>2.30397345042161e-05</v>
       </c>
       <c r="AP16" t="n">
-        <v>0.0002444628182660329</v>
+        <v>-0.0002305859267309316</v>
       </c>
       <c r="AQ16" t="n">
-        <v>-0.0004010216038687176</v>
+        <v>-7.676493391619687e-06</v>
       </c>
       <c r="AR16" t="n">
-        <v>7.133973243068994e-05</v>
+        <v>0.0001707335949599321</v>
       </c>
       <c r="AS16" t="n">
-        <v>9.283727904658188e-05</v>
+        <v>4.288379770602197e-05</v>
       </c>
       <c r="AT16" t="n">
-        <v>0.000203597807405603</v>
+        <v>-0.0002023575145804124</v>
       </c>
       <c r="AU16" t="n">
-        <v>-0.0003438838005736204</v>
+        <v>-2.8840304993375e-06</v>
       </c>
       <c r="AV16" t="n">
-        <v>5.113010050716808e-05</v>
+        <v>0.0001533864352618064</v>
       </c>
       <c r="AW16" t="n">
-        <v>0.0001051058543844435</v>
+        <v>3.983948602330101e-05</v>
       </c>
       <c r="AX16" t="n">
-        <v>-0.0006748241701191055</v>
+        <v>0.0001594425700768687</v>
       </c>
       <c r="AY16" t="n">
-        <v>0.0003646681919455549</v>
+        <v>-6.271483753174544e-05</v>
       </c>
       <c r="AZ16" t="n">
-        <v>0.0001947409761920276</v>
+        <v>-2.745786114883133e-05</v>
       </c>
       <c r="BA16" t="n">
-        <v>1.555615497352041e-05</v>
+        <v>-2.58022146100628e-05</v>
       </c>
       <c r="BB16" t="n">
-        <v>-0.0005526652965100798</v>
+        <v>0.0001395704320665578</v>
       </c>
       <c r="BC16" t="n">
-        <v>0.0003358789764750778</v>
+        <v>-6.944265506908824e-05</v>
       </c>
       <c r="BD16" t="n">
-        <v>0.0002047805413076573</v>
+        <v>-2.65116009081893e-05</v>
       </c>
       <c r="BE16" t="n">
-        <v>-3.051307395688114e-05</v>
+        <v>-3.2987028249834e-05</v>
       </c>
       <c r="BF16" t="n">
-        <v>-0.0004725934012406942</v>
+        <v>0.0001303618711053087</v>
       </c>
       <c r="BG16" t="n">
-        <v>0.0003004052208258338</v>
+        <v>-7.035803289000637e-05</v>
       </c>
       <c r="BH16" t="n">
-        <v>0.0002014713609796367</v>
+        <v>-2.062965602868131e-05</v>
       </c>
       <c r="BI16" t="n">
-        <v>-6.477199607115762e-05</v>
+        <v>-3.580223137803959e-05</v>
       </c>
       <c r="BJ16" t="n">
-        <v>-0.0004043887779086576</v>
+        <v>0.0001244436778162422</v>
       </c>
       <c r="BK16" t="n">
-        <v>0.0002718675192607903</v>
+        <v>-6.983709384066289e-05</v>
       </c>
       <c r="BL16" t="n">
-        <v>0.0001930787607812153</v>
+        <v>-1.44794592640089e-05</v>
       </c>
       <c r="BM16" t="n">
-        <v>-8.979418418545809e-05</v>
+        <v>-3.804509305107701e-05</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Russia</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.000723789783913524</v>
+        <v>-0.01247208884926686</v>
       </c>
       <c r="C17" t="n">
-        <v>5.337551159147233e-05</v>
+        <v>-0.00259761964084626</v>
       </c>
       <c r="D17" t="n">
-        <v>3.512206109297829e-06</v>
+        <v>0.002638595304687448</v>
       </c>
       <c r="E17" t="n">
-        <v>1.190632137910052e-09</v>
+        <v>0.0009920467579371678</v>
       </c>
       <c r="F17" t="n">
-        <v>-1.397434351554525e-07</v>
+        <v>0.001216174927293032</v>
       </c>
       <c r="G17" t="n">
-        <v>-8.503050745970242e-08</v>
+        <v>0.0002624441670718364</v>
       </c>
       <c r="H17" t="n">
-        <v>-4.612112489947368e-08</v>
+        <v>-0.0006720277498249276</v>
       </c>
       <c r="I17" t="n">
-        <v>-2.464715724395904e-08</v>
+        <v>-0.0004875059774716816</v>
       </c>
       <c r="J17" t="n">
-        <v>-1.314422907094899e-08</v>
+        <v>-8.083789496883309e-05</v>
       </c>
       <c r="K17" t="n">
-        <v>-7.007726464997723e-09</v>
+        <v>9.176121959758774e-05</v>
       </c>
       <c r="L17" t="n">
-        <v>-3.735952969871812e-09</v>
+        <v>0.0001698980105675226</v>
       </c>
       <c r="M17" t="n">
-        <v>-1.991696498388372e-09</v>
+        <v>-3.311562280129565e-05</v>
       </c>
       <c r="N17" t="n">
-        <v>-1.061804514380514e-09</v>
+        <v>-1.537541308267224e-05</v>
       </c>
       <c r="O17" t="n">
-        <v>-5.660645079103802e-10</v>
+        <v>1.431132176642492e-05</v>
       </c>
       <c r="P17" t="n">
-        <v>-3.017777920861969e-10</v>
+        <v>2.286913359563256e-05</v>
       </c>
       <c r="Q17" t="n">
-        <v>-1.608824335711787e-10</v>
+        <v>-9.53394647484344e-05</v>
       </c>
       <c r="R17" t="n">
-        <v>-1.459646503581326e-05</v>
+        <v>0.0002002638726802537</v>
       </c>
       <c r="S17" t="n">
-        <v>5.720428061091758e-06</v>
+        <v>-2.213630224083552e-05</v>
       </c>
       <c r="T17" t="n">
-        <v>4.062565534814152e-06</v>
+        <v>-6.800807606188626e-05</v>
       </c>
       <c r="U17" t="n">
-        <v>2.241805399288638e-06</v>
+        <v>-9.741205056791617e-05</v>
       </c>
       <c r="V17" t="n">
-        <v>1.200841944617782e-06</v>
+        <v>2.798086190531927e-05</v>
       </c>
       <c r="W17" t="n">
-        <v>6.406151719115035e-07</v>
+        <v>8.424003184928677e-06</v>
       </c>
       <c r="X17" t="n">
-        <v>3.415539922658561e-07</v>
+        <v>1.520301477943099e-05</v>
       </c>
       <c r="Y17" t="n">
-        <v>1.820901511690555e-07</v>
+        <v>-5.812359905015329e-05</v>
       </c>
       <c r="Z17" t="n">
-        <v>9.707527159292597e-08</v>
+        <v>4.525870483142159e-05</v>
       </c>
       <c r="AA17" t="n">
-        <v>5.175235032189647e-08</v>
+        <v>4.31399635195741e-06</v>
       </c>
       <c r="AB17" t="n">
-        <v>2.758998370569106e-08</v>
+        <v>2.254414589747095e-06</v>
       </c>
       <c r="AC17" t="n">
-        <v>1.470864940538075e-08</v>
+        <v>-5.993076396724966e-05</v>
       </c>
       <c r="AD17" t="n">
-        <v>7.841409718639324e-09</v>
+        <v>4.564605490101856e-05</v>
       </c>
       <c r="AE17" t="n">
-        <v>4.180377452911712e-09</v>
+        <v>8.175044173947464e-06</v>
       </c>
       <c r="AF17" t="n">
-        <v>2.228624223745305e-09</v>
+        <v>5.593691593324939e-06</v>
       </c>
       <c r="AG17" t="n">
-        <v>1.188114228092796e-09</v>
+        <v>-5.75028671031397e-05</v>
       </c>
       <c r="AH17" t="n">
-        <v>1.147046921577e-05</v>
+        <v>-0.001256261703832377</v>
       </c>
       <c r="AI17" t="n">
-        <v>1.244133414807385e-05</v>
+        <v>-0.0008740648352823547</v>
       </c>
       <c r="AJ17" t="n">
-        <v>7.10726108042742e-06</v>
+        <v>-7.418262798252811e-05</v>
       </c>
       <c r="AK17" t="n">
-        <v>3.824595109534211e-06</v>
+        <v>0.0003027655472340206</v>
       </c>
       <c r="AL17" t="n">
-        <v>2.041622098937219e-06</v>
+        <v>-0.0005449009143138616</v>
       </c>
       <c r="AM17" t="n">
-        <v>1.088620862882315e-06</v>
+        <v>-0.0001984661406391989</v>
       </c>
       <c r="AN17" t="n">
-        <v>5.803757417881756e-07</v>
+        <v>0.0002101150711138262</v>
       </c>
       <c r="AO17" t="n">
-        <v>3.094084603084102e-07</v>
+        <v>0.0003614353137033742</v>
       </c>
       <c r="AP17" t="n">
-        <v>1.649505459949991e-07</v>
+        <v>-0.0005285302493241101</v>
       </c>
       <c r="AQ17" t="n">
-        <v>8.793770734610781e-08</v>
+        <v>-0.0002020825545661648</v>
       </c>
       <c r="AR17" t="n">
-        <v>4.688095966625943e-08</v>
+        <v>0.0002347523294704575</v>
       </c>
       <c r="AS17" t="n">
-        <v>2.499296861810585e-08</v>
+        <v>0.0004065816175649672</v>
       </c>
       <c r="AT17" t="n">
-        <v>1.332414020586062e-08</v>
+        <v>-0.0004701207687498053</v>
       </c>
       <c r="AU17" t="n">
-        <v>7.10330633017084e-09</v>
+        <v>-0.0001832008749232752</v>
       </c>
       <c r="AV17" t="n">
-        <v>3.786883058827668e-09</v>
+        <v>0.0002286744828867091</v>
       </c>
       <c r="AW17" t="n">
-        <v>2.018846243512917e-09</v>
+        <v>0.0003994082600885816</v>
       </c>
       <c r="AX17" t="n">
-        <v>-0.0001861341407346146</v>
+        <v>-0.0004548468475511107</v>
       </c>
       <c r="AY17" t="n">
-        <v>-9.94879078076802e-05</v>
+        <v>0.0001590320777461168</v>
       </c>
       <c r="AZ17" t="n">
-        <v>-5.305782341219773e-05</v>
+        <v>9.964096594063287e-05</v>
       </c>
       <c r="BA17" t="n">
-        <v>-2.828739652716761e-05</v>
+        <v>6.237090350537208e-05</v>
       </c>
       <c r="BB17" t="n">
-        <v>-1.508055941462212e-05</v>
+        <v>-0.0004074161715356444</v>
       </c>
       <c r="BC17" t="n">
-        <v>-8.039688858987654e-06</v>
+        <v>0.0001728257074874928</v>
       </c>
       <c r="BD17" t="n">
-        <v>-4.286083755819537e-06</v>
+        <v>0.0001177684775808738</v>
       </c>
       <c r="BE17" t="n">
-        <v>-2.284977943288148e-06</v>
+        <v>7.989876589982197e-05</v>
       </c>
       <c r="BF17" t="n">
-        <v>-1.218157275696945e-06</v>
+        <v>-0.0003838305218304846</v>
       </c>
       <c r="BG17" t="n">
-        <v>-6.494185858975684e-07</v>
+        <v>0.0001703822668606232</v>
       </c>
       <c r="BH17" t="n">
-        <v>-3.462151464178403e-07</v>
+        <v>0.0001195045992095789</v>
       </c>
       <c r="BI17" t="n">
-        <v>-1.845726780943726e-07</v>
+        <v>8.351151675609915e-05</v>
       </c>
       <c r="BJ17" t="n">
-        <v>-9.839856473981063e-08</v>
+        <v>-0.0003702745382049986</v>
       </c>
       <c r="BK17" t="n">
-        <v>-5.245780492980071e-08</v>
+        <v>0.0001623778177596557</v>
       </c>
       <c r="BL17" t="n">
-        <v>-2.796607151058687e-08</v>
+        <v>0.0001179953505449426</v>
       </c>
       <c r="BM17" t="n">
-        <v>-1.490914758598564e-08</v>
+        <v>8.510404194021317e-05</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>SouthAfrica</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.01129781201639208</v>
+        <v>0.0004886071866749847</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.003750672387688495</v>
+        <v>0.0001283848457481581</v>
       </c>
       <c r="D18" t="n">
-        <v>0.002158064106622794</v>
+        <v>3.406586550309955e-05</v>
       </c>
       <c r="E18" t="n">
-        <v>0.001491596504195784</v>
+        <v>9.207381014673889e-06</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.000304332099853026</v>
+        <v>2.573085639575122e-06</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.0004789439704000658</v>
+        <v>7.607252799301883e-07</v>
       </c>
       <c r="H18" t="n">
-        <v>-1.282572921602585e-05</v>
+        <v>2.447647361593976e-07</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0001314598047460085</v>
+        <v>8.770279430492774e-08</v>
       </c>
       <c r="J18" t="n">
-        <v>3.042860567636523e-05</v>
+        <v>3.513101090230767e-08</v>
       </c>
       <c r="K18" t="n">
-        <v>-3.057543079262467e-05</v>
+        <v>1.545034370378417e-08</v>
       </c>
       <c r="L18" t="n">
-        <v>-1.476077933801122e-05</v>
+        <v>7.253264729847675e-09</v>
       </c>
       <c r="M18" t="n">
-        <v>5.542680556365517e-06</v>
+        <v>3.543940979762612e-09</v>
       </c>
       <c r="N18" t="n">
-        <v>5.263039408915522e-06</v>
+        <v>1.770973442444183e-09</v>
       </c>
       <c r="O18" t="n">
-        <v>-4.763702841943097e-07</v>
+        <v>8.957339156397494e-10</v>
       </c>
       <c r="P18" t="n">
-        <v>-1.57025395022482e-06</v>
+        <v>4.559147783215999e-10</v>
       </c>
       <c r="Q18" t="n">
-        <v>-1.873661431387835e-07</v>
+        <v>2.328082859408469e-10</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.0005645770715270606</v>
+        <v>2.496327006937845e-06</v>
       </c>
       <c r="S18" t="n">
-        <v>0.0003021183309953039</v>
+        <v>-5.682331730421668e-07</v>
       </c>
       <c r="T18" t="n">
-        <v>0.0003742726520876313</v>
+        <v>-7.715019618252645e-07</v>
       </c>
       <c r="U18" t="n">
-        <v>-1.944201629540598e-05</v>
+        <v>-5.202035569562496e-07</v>
       </c>
       <c r="V18" t="n">
-        <v>-0.0001041285260479386</v>
+        <v>-2.990171735677575e-07</v>
       </c>
       <c r="W18" t="n">
-        <v>-1.664257147428668e-05</v>
+        <v>-1.616533375374161e-07</v>
       </c>
       <c r="X18" t="n">
-        <v>2.594155761011319e-05</v>
+        <v>-8.502246912397576e-08</v>
       </c>
       <c r="Y18" t="n">
-        <v>9.913737467874904e-06</v>
+        <v>-4.413399405905112e-08</v>
       </c>
       <c r="Z18" t="n">
-        <v>-5.226207041402771e-06</v>
+        <v>-2.276139987217152e-08</v>
       </c>
       <c r="AA18" t="n">
-        <v>-3.843943136011078e-06</v>
+        <v>-1.170085283787316e-08</v>
       </c>
       <c r="AB18" t="n">
-        <v>6.780751532796277e-07</v>
+        <v>-6.005195791404332e-09</v>
       </c>
       <c r="AC18" t="n">
-        <v>1.214184479316006e-06</v>
+        <v>-3.079487157512642e-09</v>
       </c>
       <c r="AD18" t="n">
-        <v>5.821836531727477e-08</v>
+        <v>-1.578512625787981e-09</v>
       </c>
       <c r="AE18" t="n">
-        <v>-3.279285778987807e-07</v>
+        <v>-8.089574243695408e-10</v>
       </c>
       <c r="AF18" t="n">
-        <v>-8.32643006229574e-08</v>
+        <v>-4.14530578592058e-10</v>
       </c>
       <c r="AG18" t="n">
-        <v>7.477224194626928e-08</v>
+        <v>-2.124045354437271e-10</v>
       </c>
       <c r="AH18" t="n">
-        <v>-0.0004656474233849604</v>
+        <v>9.287828073714382e-06</v>
       </c>
       <c r="AI18" t="n">
-        <v>-0.0002385255865849153</v>
+        <v>1.406487635531341e-05</v>
       </c>
       <c r="AJ18" t="n">
-        <v>2.078972274810803e-05</v>
+        <v>9.626318550134779e-06</v>
       </c>
       <c r="AK18" t="n">
-        <v>7.588071470848605e-05</v>
+        <v>5.561490172935452e-06</v>
       </c>
       <c r="AL18" t="n">
-        <v>7.818379039415234e-06</v>
+        <v>3.013165776322726e-06</v>
       </c>
       <c r="AM18" t="n">
-        <v>-1.930261675328244e-05</v>
+        <v>1.586402440051808e-06</v>
       </c>
       <c r="AN18" t="n">
-        <v>-6.211235135160237e-06</v>
+        <v>8.238878273427711e-07</v>
       </c>
       <c r="AO18" t="n">
-        <v>4.150944957357818e-06</v>
+        <v>4.25011697065221e-07</v>
       </c>
       <c r="AP18" t="n">
-        <v>2.582219085262826e-06</v>
+        <v>2.185109592522193e-07</v>
       </c>
       <c r="AQ18" t="n">
-        <v>-6.335220994128412e-07</v>
+        <v>1.121527792101218e-07</v>
       </c>
       <c r="AR18" t="n">
-        <v>-8.522534149296273e-07</v>
+        <v>5.751419105251429e-08</v>
       </c>
       <c r="AS18" t="n">
-        <v>3.291636492048402e-09</v>
+        <v>2.9481640605523e-08</v>
       </c>
       <c r="AT18" t="n">
-        <v>2.391831361992723e-07</v>
+        <v>1.510889793858584e-08</v>
       </c>
       <c r="AU18" t="n">
-        <v>4.792837243806067e-08</v>
+        <v>7.742219648934273e-09</v>
       </c>
       <c r="AV18" t="n">
-        <v>-5.715229777192262e-08</v>
+        <v>3.967104234113454e-09</v>
       </c>
       <c r="AW18" t="n">
-        <v>-2.508563611103822e-08</v>
+        <v>2.032681165518262e-09</v>
       </c>
       <c r="AX18" t="n">
-        <v>8.65852086728806e-05</v>
+        <v>-4.283023336123716e-05</v>
       </c>
       <c r="AY18" t="n">
-        <v>-1.985081832440554e-05</v>
+        <v>-2.180392914491935e-05</v>
       </c>
       <c r="AZ18" t="n">
-        <v>2.096914348264309e-05</v>
+        <v>-1.113500356050127e-05</v>
       </c>
       <c r="BA18" t="n">
-        <v>2.765628338221829e-06</v>
+        <v>-5.695699050045989e-06</v>
       </c>
       <c r="BB18" t="n">
-        <v>-3.397483427823654e-06</v>
+        <v>-2.91582092387228e-06</v>
       </c>
       <c r="BC18" t="n">
-        <v>-1.855720689008862e-06</v>
+        <v>-1.493331623091798e-06</v>
       </c>
       <c r="BD18" t="n">
-        <v>6.602654985352343e-07</v>
+        <v>-7.649691648059772e-07</v>
       </c>
       <c r="BE18" t="n">
-        <v>6.350025691244352e-07</v>
+        <v>-3.919028667985148e-07</v>
       </c>
       <c r="BF18" t="n">
-        <v>-5.084864263971351e-08</v>
+        <v>-2.007875270724512e-07</v>
       </c>
       <c r="BG18" t="n">
-        <v>-1.890377156836957e-07</v>
+        <v>-1.028743470060837e-07</v>
       </c>
       <c r="BH18" t="n">
-        <v>-2.416937281539293e-08</v>
+        <v>-5.270885454377946e-08</v>
       </c>
       <c r="BI18" t="n">
-        <v>4.792449340720134e-08</v>
+        <v>-2.700618101856199e-08</v>
       </c>
       <c r="BJ18" t="n">
-        <v>1.656174732145007e-08</v>
+        <v>-1.383707670296621e-08</v>
       </c>
       <c r="BK18" t="n">
-        <v>-1.003246554819092e-08</v>
+        <v>-7.089674938789731e-09</v>
       </c>
       <c r="BL18" t="n">
-        <v>-6.683544751776286e-09</v>
+        <v>-3.632525775383655e-09</v>
       </c>
       <c r="BM18" t="n">
-        <v>1.442717313373361e-09</v>
+        <v>-1.861192493354593e-09</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.01340195179942198</v>
+        <v>-0.002684837924965605</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.00215910423311057</v>
+        <v>-0.001030210162049437</v>
       </c>
       <c r="D19" t="n">
-        <v>0.004320808062186363</v>
+        <v>0.0005409276678340413</v>
       </c>
       <c r="E19" t="n">
-        <v>0.001239627817110118</v>
+        <v>0.0007093285178104128</v>
       </c>
       <c r="F19" t="n">
-        <v>3.44205137102013e-05</v>
+        <v>0.0006818069730132979</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0008204165520472403</v>
+        <v>-0.0004703228548317074</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.0002700300836826422</v>
+        <v>-0.000745735711351515</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.0005316160576060891</v>
+        <v>-0.0005223794993428616</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.0006767830446146051</v>
+        <v>0.0003737394419430133</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0003289585658482285</v>
+        <v>0.0003169856492798228</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0003543857914316529</v>
+        <v>0.0001086798641678745</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0001741995960301874</v>
+        <v>-0.0003199297818909044</v>
       </c>
       <c r="N19" t="n">
-        <v>-0.0003995763720469457</v>
+        <v>-5.124044986039787e-05</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0001072739186662811</v>
+        <v>-0.0001103777368566666</v>
       </c>
       <c r="P19" t="n">
-        <v>4.241800913070983e-05</v>
+        <v>5.035627457225896e-05</v>
       </c>
       <c r="Q19" t="n">
-        <v>9.729781752616009e-05</v>
+        <v>-4.115054699897561e-05</v>
       </c>
       <c r="R19" t="n">
-        <v>0.0001142886858605279</v>
+        <v>-0.0005773481470784791</v>
       </c>
       <c r="S19" t="n">
-        <v>-0.0002334590476133944</v>
+        <v>0.000113098764525269</v>
       </c>
       <c r="T19" t="n">
-        <v>-3.429228997985494e-05</v>
+        <v>0.0002769120813254084</v>
       </c>
       <c r="U19" t="n">
-        <v>-0.0001376930675648804</v>
+        <v>0.0002176618141737224</v>
       </c>
       <c r="V19" t="n">
-        <v>0.0005037309300786058</v>
+        <v>-8.099160497194758e-05</v>
       </c>
       <c r="W19" t="n">
-        <v>-3.924766517760296e-05</v>
+        <v>-3.651465845362142e-05</v>
       </c>
       <c r="X19" t="n">
-        <v>-6.958059501682217e-05</v>
+        <v>-6.767072253423078e-05</v>
       </c>
       <c r="Y19" t="n">
-        <v>-0.0002091360895161582</v>
+        <v>2.859694645355165e-05</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.0002578039087886762</v>
+        <v>-2.971569119001488e-05</v>
       </c>
       <c r="AA19" t="n">
-        <v>-7.380443774571235e-05</v>
+        <v>0.0001224798401115482</v>
       </c>
       <c r="AB19" t="n">
-        <v>3.397037461428601e-05</v>
+        <v>3.093387646007566e-05</v>
       </c>
       <c r="AC19" t="n">
-        <v>-0.0001452533319372399</v>
+        <v>-1.21726315035291e-05</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.0001766890213592016</v>
+        <v>-0.0001213941460409097</v>
       </c>
       <c r="AE19" t="n">
-        <v>-7.458922031190261e-05</v>
+        <v>4.99154435874827e-05</v>
       </c>
       <c r="AF19" t="n">
-        <v>5.275247763382585e-05</v>
+        <v>4.46961529117875e-05</v>
       </c>
       <c r="AG19" t="n">
-        <v>-0.0001221796534716068</v>
+        <v>4.151268222401253e-05</v>
       </c>
       <c r="AH19" t="n">
-        <v>-6.580829577023781e-05</v>
+        <v>-0.001040146206837731</v>
       </c>
       <c r="AI19" t="n">
-        <v>-0.0007363228526325701</v>
+        <v>-0.0003562948433662743</v>
       </c>
       <c r="AJ19" t="n">
-        <v>-0.000196575159803734</v>
+        <v>-8.294279399410485e-05</v>
       </c>
       <c r="AK19" t="n">
-        <v>0.0001981667385002265</v>
+        <v>0.0003811850832178101</v>
       </c>
       <c r="AL19" t="n">
-        <v>0.000530052428104713</v>
+        <v>-0.0006883464522176652</v>
       </c>
       <c r="AM19" t="n">
-        <v>-0.000246549695441277</v>
+        <v>-0.0001202505060505328</v>
       </c>
       <c r="AN19" t="n">
-        <v>-0.0001442107370915589</v>
+        <v>-2.1750533690804e-05</v>
       </c>
       <c r="AO19" t="n">
-        <v>-5.738948063004866e-05</v>
+        <v>0.0003175771916211763</v>
       </c>
       <c r="AP19" t="n">
-        <v>0.0002601067252402717</v>
+        <v>-0.0005744357078888721</v>
       </c>
       <c r="AQ19" t="n">
-        <v>-0.0001642485840309623</v>
+        <v>-4.030276892064774e-05</v>
       </c>
       <c r="AR19" t="n">
-        <v>-1.395338895941474e-05</v>
+        <v>6.178545324442914e-05</v>
       </c>
       <c r="AS19" t="n">
-        <v>-5.23110844716494e-05</v>
+        <v>0.0003420260482801652</v>
       </c>
       <c r="AT19" t="n">
-        <v>0.0001858774959933383</v>
+        <v>-0.0004804002394411688</v>
       </c>
       <c r="AU19" t="n">
-        <v>-0.0001143103217580227</v>
+        <v>-4.612055924124274e-05</v>
       </c>
       <c r="AV19" t="n">
-        <v>1.435799618851657e-05</v>
+        <v>5.169321626193795e-05</v>
       </c>
       <c r="AW19" t="n">
-        <v>-7.011151867722117e-05</v>
+        <v>0.0003269560747704425</v>
       </c>
       <c r="AX19" t="n">
-        <v>-0.0004264667967940048</v>
+        <v>0.0003797286489191955</v>
       </c>
       <c r="AY19" t="n">
-        <v>5.77292331510995e-05</v>
+        <v>-0.0001576335622625486</v>
       </c>
       <c r="AZ19" t="n">
-        <v>-1.837911910455632e-05</v>
+        <v>-5.710439578717554e-05</v>
       </c>
       <c r="BA19" t="n">
-        <v>0.0001000381288411034</v>
+        <v>1.754753222002368e-05</v>
       </c>
       <c r="BB19" t="n">
-        <v>-0.0002178869855760796</v>
+        <v>0.0003211407345764097</v>
       </c>
       <c r="BC19" t="n">
-        <v>8.627766153731088e-05</v>
+        <v>-0.0001432468515826733</v>
       </c>
       <c r="BD19" t="n">
-        <v>-3.784954780883978e-05</v>
+        <v>-7.880721077708461e-05</v>
       </c>
       <c r="BE19" t="n">
-        <v>9.977981017687423e-05</v>
+        <v>-1.951433371021851e-05</v>
       </c>
       <c r="BF19" t="n">
-        <v>-0.0001485039658908128</v>
+        <v>0.0002684943928917021</v>
       </c>
       <c r="BG19" t="n">
-        <v>7.575048552442566e-05</v>
+        <v>-0.0001205780760755438</v>
       </c>
       <c r="BH19" t="n">
-        <v>-4.925874690211417e-05</v>
+        <v>-6.7762345778202e-05</v>
       </c>
       <c r="BI19" t="n">
-        <v>9.030254526872171e-05</v>
+        <v>-2.638520243591225e-05</v>
       </c>
       <c r="BJ19" t="n">
-        <v>-0.0001054289674749679</v>
+        <v>0.0002248632769197115</v>
       </c>
       <c r="BK19" t="n">
-        <v>6.630138853474988e-05</v>
+        <v>-0.0001096884166562223</v>
       </c>
       <c r="BL19" t="n">
-        <v>-5.373156436809087e-05</v>
+        <v>-6.300118544566062e-05</v>
       </c>
       <c r="BM19" t="n">
-        <v>7.582441429277511e-05</v>
+        <v>-2.708541722459698e-05</v>
       </c>
     </row>
     <row r="20">

</xml_diff>